<commit_message>
implemented popout log for application
</commit_message>
<xml_diff>
--- a/resources/Dose_Response_Library.xlsx
+++ b/resources/Dose_Response_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scaainc-my.sharepoint.com/personal/jmozier_scainc_com/Documents/Projects/RIS-409 to 104 RTR  NATA (2013-2017)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Lindsey\OneDrive - SC&amp;A, Inc\HEM4Python\Version_Master\HEM4\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E099FF3-ADCF-4757-83F0-947B813D6E9F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31184AE9-D6E8-43E9-838E-8A8FA90F3997}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="4110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="2700" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dose Response Value Library" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,15 @@
     <definedName name="Z_E392D6CB_6FB5_47D6_BFF9_30F47B865CA7_.wvu.PrintArea" localSheetId="0" hidden="1">'Dose Response Value Library'!$A$1:$U$472</definedName>
     <definedName name="Z_E392D6CB_6FB5_47D6_BFF9_30F47B865CA7_.wvu.PrintTitles" localSheetId="0" hidden="1">'Dose Response Value Library'!$A:$A,'Dose Response Value Library'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2576,12 +2584,6 @@
   </si>
   <si>
     <t>RfC = antimony trioxide. ERPG2 updated 1/2017. MRL = antimony trioxide</t>
-  </si>
-  <si>
-    <t>1,2,3,4,6,7,8,9-Octachlorodibenzo-p-dioxin</t>
-  </si>
-  <si>
-    <t>1,2,3,4,6,7,8,9-Octachlorodibenzofuran</t>
   </si>
   <si>
     <t>2-Methylphenanthrene</t>
@@ -2644,6 +2646,12 @@
   </si>
   <si>
     <t>URE = 0.001xBaP based on EPA RPF which does not coorespond to a POM group - removed from group 7 5/2018. POM group 7 adjusted URE updated 4/2017.</t>
+  </si>
+  <si>
+    <t>1,2,3,4,6,7,8,9-Octochlorodibenzo-p-dioxin</t>
+  </si>
+  <si>
+    <t>1,2,3,4,6,7,8,9-Octochlorodibenzofuran</t>
   </si>
 </sst>
 </file>
@@ -3696,13 +3704,13 @@
   <dimension ref="A1:X498"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
@@ -4320,7 +4328,7 @@
         <v>742</v>
       </c>
       <c r="R15" s="13" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="U15" s="1">
         <f t="shared" si="0"/>
@@ -4830,7 +4838,7 @@
       <c r="P29" s="12"/>
       <c r="Q29" s="13"/>
       <c r="R29" s="13" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="U29" s="1">
         <f t="shared" si="0"/>
@@ -4884,7 +4892,7 @@
         <v>741</v>
       </c>
       <c r="R30" s="13" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="U30" s="1">
         <f t="shared" si="0"/>
@@ -5160,7 +5168,7 @@
       <c r="P38" s="12"/>
       <c r="Q38" s="13"/>
       <c r="R38" s="13" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="U38" s="1">
         <f t="shared" si="0"/>
@@ -5510,7 +5518,7 @@
         <v>741</v>
       </c>
       <c r="R47" s="55" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="U47" s="1">
         <f t="shared" si="0"/>
@@ -6423,7 +6431,7 @@
         <v>759</v>
       </c>
       <c r="R69" s="56" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="U69" s="1">
         <f t="shared" si="1"/>
@@ -9163,7 +9171,7 @@
       <c r="P142" s="12"/>
       <c r="Q142" s="13"/>
       <c r="R142" s="13" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="U142" s="1">
         <f>MIN(F142:P142)</f>
@@ -10884,7 +10892,7 @@
     </row>
     <row r="188" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A188" s="10" t="s">
-        <v>839</v>
+        <v>856</v>
       </c>
       <c r="B188" s="10" t="s">
         <v>747</v>
@@ -10928,7 +10936,7 @@
     </row>
     <row r="189" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A189" s="10" t="s">
-        <v>840</v>
+        <v>857</v>
       </c>
       <c r="B189" s="10" t="s">
         <v>747</v>
@@ -12296,7 +12304,7 @@
         <v>48</v>
       </c>
       <c r="R221" s="13" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="U221" s="1">
         <f>MIN(F221:P221)</f>
@@ -12374,7 +12382,7 @@
         <v>336</v>
       </c>
       <c r="R223" s="13" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="U223" s="1">
         <f t="shared" si="3"/>
@@ -15921,7 +15929,7 @@
       <c r="P315" s="12"/>
       <c r="Q315" s="13"/>
       <c r="R315" s="13" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="U315" s="1">
         <f t="shared" si="4"/>
@@ -17402,13 +17410,13 @@
     </row>
     <row r="357" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A357" s="10" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B357" s="10" t="s">
         <v>531</v>
       </c>
       <c r="C357" s="51" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="D357" s="12">
         <v>4.8000000000000001E-5</v>
@@ -17426,10 +17434,10 @@
       <c r="O357" s="12"/>
       <c r="P357" s="12"/>
       <c r="Q357" s="13" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="R357" s="13" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="358" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
@@ -18887,7 +18895,7 @@
         <v>591</v>
       </c>
       <c r="R399" s="13" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="U399" s="1">
         <f t="shared" si="7"/>
@@ -19589,7 +19597,7 @@
         <v>623</v>
       </c>
       <c r="B419" s="10" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C419" s="11">
         <v>218019</v>
@@ -19613,7 +19621,7 @@
       <c r="P419" s="12"/>
       <c r="Q419" s="13"/>
       <c r="R419" s="13" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="U419" s="1">
         <f>MIN(F419:P419)</f>

</xml_diff>

<commit_message>
added validation for DoseResponse and TargetOrganEndpoints. Also updated the data files themselves to resolve missing pollutants
</commit_message>
<xml_diff>
--- a/resources/Dose_Response_Library.xlsx
+++ b/resources/Dose_Response_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scaainc-my.sharepoint.com/personal/jmozier_scainc_com/Documents/Projects/RIS-409 to 104 RTR  NATA (2013-2017)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Stolte\IdeaProjects\HEM4\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CFFCE8C-70D8-4F08-A766-9B1C23AC6A59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE32B69-345D-4F5C-9ACB-418F81B927D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="4110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="528" yWindow="792" windowWidth="22380" windowHeight="11424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dose Response Value Library" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3712,35 +3714,35 @@
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A328" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G349" sqref="G349"/>
+      <selection pane="bottomLeft" activeCell="A334" sqref="A334:XFD334"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="8" customWidth="1"/>
-    <col min="10" max="11" width="9.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" style="8" customWidth="1"/>
+    <col min="10" max="11" width="9.6640625" style="8" customWidth="1"/>
     <col min="12" max="12" width="10" style="8" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="8" customWidth="1"/>
-    <col min="14" max="15" width="9.28515625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="8" customWidth="1"/>
+    <col min="14" max="15" width="9.33203125" style="8" customWidth="1"/>
     <col min="16" max="16" width="11" style="8" customWidth="1"/>
     <col min="17" max="17" width="24" style="9" customWidth="1"/>
-    <col min="18" max="18" width="34.7109375" style="9" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="34.6640625" style="9" customWidth="1"/>
+    <col min="19" max="19" width="10.88671875" style="1" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9.109375" style="1" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="13" style="9" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="23" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3805,7 +3807,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
@@ -3859,7 +3861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
@@ -3893,7 +3895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>25</v>
       </c>
@@ -3927,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>26</v>
       </c>
@@ -3967,7 +3969,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>27</v>
       </c>
@@ -4001,7 +4003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>29</v>
       </c>
@@ -4036,7 +4038,7 @@
       </c>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>30</v>
       </c>
@@ -4071,7 +4073,7 @@
       </c>
       <c r="X8" s="3"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>31</v>
       </c>
@@ -4106,7 +4108,7 @@
       </c>
       <c r="X9" s="3"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>32</v>
       </c>
@@ -4140,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>33</v>
       </c>
@@ -4174,7 +4176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>35</v>
       </c>
@@ -4208,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
@@ -4252,7 +4254,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
@@ -4292,7 +4294,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>38</v>
       </c>
@@ -4342,7 +4344,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>39</v>
       </c>
@@ -4376,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>40</v>
       </c>
@@ -4410,7 +4412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>41</v>
       </c>
@@ -4446,7 +4448,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>43</v>
       </c>
@@ -4480,7 +4482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>45</v>
       </c>
@@ -4530,7 +4532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>47</v>
       </c>
@@ -4562,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>49</v>
       </c>
@@ -4596,7 +4598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>50</v>
       </c>
@@ -4630,7 +4632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>51</v>
       </c>
@@ -4664,7 +4666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>53</v>
       </c>
@@ -4698,7 +4700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>54</v>
       </c>
@@ -4732,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>55</v>
       </c>
@@ -4766,7 +4768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>57</v>
       </c>
@@ -4800,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>58</v>
       </c>
@@ -4852,7 +4854,7 @@
         <v>7.1000000000000005E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>59</v>
       </c>
@@ -4906,7 +4908,7 @@
         <v>7.1000000000000005E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>60</v>
       </c>
@@ -4938,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>61</v>
       </c>
@@ -4972,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>62</v>
       </c>
@@ -5006,7 +5008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>63</v>
       </c>
@@ -5040,7 +5042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>64</v>
       </c>
@@ -5074,7 +5076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>65</v>
       </c>
@@ -5108,7 +5110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>66</v>
       </c>
@@ -5142,7 +5144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>67</v>
       </c>
@@ -5182,7 +5184,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>69</v>
       </c>
@@ -5216,7 +5218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>71</v>
       </c>
@@ -5248,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>72</v>
       </c>
@@ -5280,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>73</v>
       </c>
@@ -5314,7 +5316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>74</v>
       </c>
@@ -5366,7 +5368,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>75</v>
       </c>
@@ -5400,7 +5402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>76</v>
       </c>
@@ -5444,7 +5446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>77</v>
       </c>
@@ -5478,7 +5480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A47" s="52" t="s">
         <v>78</v>
       </c>
@@ -5532,7 +5534,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>79</v>
       </c>
@@ -5568,7 +5570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>81</v>
       </c>
@@ -5620,7 +5622,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>82</v>
       </c>
@@ -5668,7 +5670,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>83</v>
       </c>
@@ -5716,7 +5718,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>84</v>
       </c>
@@ -5760,7 +5762,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>85</v>
       </c>
@@ -5796,7 +5798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>87</v>
       </c>
@@ -5834,7 +5836,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>88</v>
       </c>
@@ -5872,7 +5874,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>90</v>
       </c>
@@ -5910,7 +5912,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>93</v>
       </c>
@@ -5948,7 +5950,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>94</v>
       </c>
@@ -5986,7 +5988,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>95</v>
       </c>
@@ -6024,7 +6026,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>96</v>
       </c>
@@ -6068,7 +6070,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>98</v>
       </c>
@@ -6106,7 +6108,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>99</v>
       </c>
@@ -6146,7 +6148,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
         <v>102</v>
       </c>
@@ -6186,7 +6188,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>104</v>
       </c>
@@ -6226,7 +6228,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="35" t="s">
         <v>106</v>
       </c>
@@ -6265,7 +6267,7 @@
       </c>
       <c r="V65" s="45"/>
     </row>
-    <row r="66" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>109</v>
       </c>
@@ -6305,7 +6307,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>112</v>
       </c>
@@ -6349,7 +6351,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>113</v>
       </c>
@@ -6393,7 +6395,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>115</v>
       </c>
@@ -6445,7 +6447,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>116</v>
       </c>
@@ -6481,7 +6483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>118</v>
       </c>
@@ -6515,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>119</v>
       </c>
@@ -6555,7 +6557,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>120</v>
       </c>
@@ -6593,7 +6595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>121</v>
       </c>
@@ -6629,7 +6631,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>124</v>
       </c>
@@ -6667,7 +6669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>126</v>
       </c>
@@ -6705,7 +6707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>128</v>
       </c>
@@ -6743,7 +6745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>132</v>
       </c>
@@ -6775,7 +6777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>133</v>
       </c>
@@ -6815,7 +6817,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>134</v>
       </c>
@@ -6849,7 +6851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
         <v>135</v>
       </c>
@@ -6891,7 +6893,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
         <v>136</v>
       </c>
@@ -6925,7 +6927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="25" t="s">
         <v>137</v>
       </c>
@@ -6963,7 +6965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>138</v>
       </c>
@@ -7011,7 +7013,7 @@
         <v>3.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>140</v>
       </c>
@@ -7043,7 +7045,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>142</v>
       </c>
@@ -7081,7 +7083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="25" t="s">
         <v>143</v>
       </c>
@@ -7119,7 +7121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A88" s="25" t="s">
         <v>144</v>
       </c>
@@ -7157,7 +7159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>146</v>
       </c>
@@ -7191,7 +7193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>147</v>
       </c>
@@ -7225,7 +7227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
         <v>148</v>
       </c>
@@ -7277,7 +7279,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>149</v>
       </c>
@@ -7325,7 +7327,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A93" s="25" t="s">
         <v>150</v>
       </c>
@@ -7365,7 +7367,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="25" t="s">
         <v>153</v>
       </c>
@@ -7397,7 +7399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
         <v>154</v>
       </c>
@@ -7431,7 +7433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
         <v>155</v>
       </c>
@@ -7465,7 +7467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
         <v>156</v>
       </c>
@@ -7519,7 +7521,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
         <v>157</v>
       </c>
@@ -7559,7 +7561,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
         <v>158</v>
       </c>
@@ -7603,7 +7605,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
         <v>159</v>
       </c>
@@ -7637,7 +7639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
         <v>160</v>
       </c>
@@ -7685,7 +7687,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
         <v>162</v>
       </c>
@@ -7729,7 +7731,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
         <v>163</v>
       </c>
@@ -7767,7 +7769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A104" s="25" t="s">
         <v>166</v>
       </c>
@@ -7805,7 +7807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A105" s="25" t="s">
         <v>169</v>
       </c>
@@ -7843,7 +7845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="25" t="s">
         <v>170</v>
       </c>
@@ -7881,7 +7883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="38" t="s">
         <v>172</v>
       </c>
@@ -7919,7 +7921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A108" s="38" t="s">
         <v>173</v>
       </c>
@@ -7957,7 +7959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
         <v>176</v>
       </c>
@@ -7991,7 +7993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
         <v>178</v>
       </c>
@@ -8025,7 +8027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
         <v>179</v>
       </c>
@@ -8063,7 +8065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
         <v>180</v>
       </c>
@@ -8097,7 +8099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="25" t="s">
         <v>181</v>
       </c>
@@ -8135,7 +8137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="38" t="s">
         <v>183</v>
       </c>
@@ -8173,7 +8175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="s">
         <v>184</v>
       </c>
@@ -8207,7 +8209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
         <v>185</v>
       </c>
@@ -8243,7 +8245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A117" s="10" t="s">
         <v>187</v>
       </c>
@@ -8277,7 +8279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A118" s="10" t="s">
         <v>167</v>
       </c>
@@ -8313,7 +8315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A119" s="10" t="s">
         <v>189</v>
       </c>
@@ -8351,7 +8353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
         <v>190</v>
       </c>
@@ -8383,7 +8385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="s">
         <v>191</v>
       </c>
@@ -8421,7 +8423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A122" s="10" t="s">
         <v>192</v>
       </c>
@@ -8459,7 +8461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123" s="25" t="s">
         <v>193</v>
       </c>
@@ -8497,7 +8499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124" s="25" t="s">
         <v>194</v>
       </c>
@@ -8535,7 +8537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125" s="25" t="s">
         <v>195</v>
       </c>
@@ -8573,7 +8575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126" s="38" t="s">
         <v>196</v>
       </c>
@@ -8611,7 +8613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A127" s="38" t="s">
         <v>197</v>
       </c>
@@ -8645,7 +8647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A128" s="25" t="s">
         <v>198</v>
       </c>
@@ -8683,7 +8685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
         <v>199</v>
       </c>
@@ -8719,7 +8721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A130" s="10" t="s">
         <v>202</v>
       </c>
@@ -8755,7 +8757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>204</v>
       </c>
@@ -8791,7 +8793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
         <v>206</v>
       </c>
@@ -8827,7 +8829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>208</v>
       </c>
@@ -8863,7 +8865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
         <v>200</v>
       </c>
@@ -8897,7 +8899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A135" s="10" t="s">
         <v>210</v>
       </c>
@@ -8935,7 +8937,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="s">
         <v>213</v>
       </c>
@@ -8971,7 +8973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="s">
         <v>214</v>
       </c>
@@ -9007,7 +9009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A138" s="10" t="s">
         <v>216</v>
       </c>
@@ -9043,7 +9045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A139" s="10" t="s">
         <v>217</v>
       </c>
@@ -9079,7 +9081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="10" t="s">
         <v>219</v>
       </c>
@@ -9115,7 +9117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A141" s="10" t="s">
         <v>220</v>
       </c>
@@ -9151,7 +9153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:21" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="10" t="s">
         <v>552</v>
       </c>
@@ -9185,7 +9187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A143" s="10" t="s">
         <v>223</v>
       </c>
@@ -9221,7 +9223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A144" s="10" t="s">
         <v>225</v>
       </c>
@@ -9257,7 +9259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A145" s="10" t="s">
         <v>226</v>
       </c>
@@ -9291,7 +9293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A146" s="10" t="s">
         <v>228</v>
       </c>
@@ -9327,7 +9329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A147" s="10" t="s">
         <v>230</v>
       </c>
@@ -9363,7 +9365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A148" s="10" t="s">
         <v>231</v>
       </c>
@@ -9399,7 +9401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A149" s="10" t="s">
         <v>232</v>
       </c>
@@ -9443,7 +9445,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A150" s="10" t="s">
         <v>233</v>
       </c>
@@ -9487,7 +9489,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A151" s="25" t="s">
         <v>235</v>
       </c>
@@ -9523,7 +9525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A152" s="10" t="s">
         <v>239</v>
       </c>
@@ -9559,7 +9561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A153" s="10" t="s">
         <v>242</v>
       </c>
@@ -9605,7 +9607,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A154" s="10" t="s">
         <v>244</v>
       </c>
@@ -9643,7 +9645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A155" s="10" t="s">
         <v>245</v>
       </c>
@@ -9679,7 +9681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156" s="10" t="s">
         <v>248</v>
       </c>
@@ -9709,7 +9711,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="10" t="s">
         <v>234</v>
       </c>
@@ -9747,7 +9749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A158" s="10" t="s">
         <v>250</v>
       </c>
@@ -9791,7 +9793,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="159" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A159" s="10" t="s">
         <v>251</v>
       </c>
@@ -9829,7 +9831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A160" s="10" t="s">
         <v>252</v>
       </c>
@@ -9869,7 +9871,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="161" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A161" s="10" t="s">
         <v>253</v>
       </c>
@@ -9905,7 +9907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A162" s="10" t="s">
         <v>255</v>
       </c>
@@ -9941,7 +9943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A163" s="10" t="s">
         <v>257</v>
       </c>
@@ -9977,7 +9979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A164" s="10" t="s">
         <v>259</v>
       </c>
@@ -10015,7 +10017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A165" s="10" t="s">
         <v>260</v>
       </c>
@@ -10065,7 +10067,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="166" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:21" ht="66" x14ac:dyDescent="0.25">
       <c r="A166" s="25" t="s">
         <v>261</v>
       </c>
@@ -10109,7 +10111,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="167" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A167" s="10" t="s">
         <v>262</v>
       </c>
@@ -10155,7 +10157,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="168" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A168" s="10" t="s">
         <v>263</v>
       </c>
@@ -10191,7 +10193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A169" s="10" t="s">
         <v>264</v>
       </c>
@@ -10227,7 +10229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A170" s="10" t="s">
         <v>266</v>
       </c>
@@ -10265,7 +10267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:21" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:21" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="10" t="s">
         <v>267</v>
       </c>
@@ -10311,7 +10313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A172" s="10" t="s">
         <v>268</v>
       </c>
@@ -10349,7 +10351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A173" s="10" t="s">
         <v>270</v>
       </c>
@@ -10387,7 +10389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
         <v>271</v>
       </c>
@@ -10425,7 +10427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A175" s="10" t="s">
         <v>272</v>
       </c>
@@ -10461,7 +10463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A176" s="10" t="s">
         <v>274</v>
       </c>
@@ -10493,7 +10495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177" s="10" t="s">
         <v>276</v>
       </c>
@@ -10527,7 +10529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178" s="10" t="s">
         <v>277</v>
       </c>
@@ -10561,7 +10563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179" s="10" t="s">
         <v>278</v>
       </c>
@@ -10595,7 +10597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A180" s="10" t="s">
         <v>279</v>
       </c>
@@ -10641,7 +10643,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A181" s="10" t="s">
         <v>280</v>
       </c>
@@ -10675,7 +10677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A182" s="10" t="s">
         <v>282</v>
       </c>
@@ -10709,7 +10711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A183" s="25" t="s">
         <v>283</v>
       </c>
@@ -10741,7 +10743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A184" s="10" t="s">
         <v>285</v>
       </c>
@@ -10787,7 +10789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A185" s="10" t="s">
         <v>286</v>
       </c>
@@ -10821,7 +10823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A186" s="10" t="s">
         <v>287</v>
       </c>
@@ -10865,7 +10867,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A187" s="25" t="s">
         <v>288</v>
       </c>
@@ -10897,7 +10899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A188" s="10" t="s">
         <v>839</v>
       </c>
@@ -10941,7 +10943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A189" s="10" t="s">
         <v>840</v>
       </c>
@@ -10985,7 +10987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A190" s="10" t="s">
         <v>291</v>
       </c>
@@ -11027,7 +11029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A191" s="10" t="s">
         <v>292</v>
       </c>
@@ -11069,7 +11071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A192" s="10" t="s">
         <v>293</v>
       </c>
@@ -11111,7 +11113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A193" s="10" t="s">
         <v>294</v>
       </c>
@@ -11153,7 +11155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A194" s="10" t="s">
         <v>295</v>
       </c>
@@ -11195,7 +11197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A195" s="10" t="s">
         <v>296</v>
       </c>
@@ -11237,7 +11239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A196" s="10" t="s">
         <v>297</v>
       </c>
@@ -11279,7 +11281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A197" s="10" t="s">
         <v>298</v>
       </c>
@@ -11321,7 +11323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A198" s="10" t="s">
         <v>299</v>
       </c>
@@ -11363,7 +11365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A199" s="10" t="s">
         <v>300</v>
       </c>
@@ -11405,7 +11407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A200" s="10" t="s">
         <v>301</v>
       </c>
@@ -11449,7 +11451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A201" s="10" t="s">
         <v>302</v>
       </c>
@@ -11491,7 +11493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A202" s="10" t="s">
         <v>303</v>
       </c>
@@ -11535,7 +11537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A203" s="10" t="s">
         <v>304</v>
       </c>
@@ -11577,7 +11579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A204" s="10" t="s">
         <v>305</v>
       </c>
@@ -11619,7 +11621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A205" s="10" t="s">
         <v>306</v>
       </c>
@@ -11663,7 +11665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A206" s="10" t="s">
         <v>309</v>
       </c>
@@ -11695,7 +11697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A207" s="10" t="s">
         <v>310</v>
       </c>
@@ -11747,7 +11749,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A208" s="10" t="s">
         <v>311</v>
       </c>
@@ -11795,7 +11797,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A209" s="10" t="s">
         <v>312</v>
       </c>
@@ -11840,7 +11842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A210" s="10" t="s">
         <v>313</v>
       </c>
@@ -11876,7 +11878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A211" s="10" t="s">
         <v>315</v>
       </c>
@@ -11912,7 +11914,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A212" s="10" t="s">
         <v>316</v>
       </c>
@@ -11956,7 +11958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="213" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A213" s="10" t="s">
         <v>317</v>
       </c>
@@ -11994,7 +11996,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="214" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214" s="10" t="s">
         <v>318</v>
       </c>
@@ -12030,7 +12032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="10" t="s">
         <v>319</v>
       </c>
@@ -12070,7 +12072,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A216" s="10" t="s">
         <v>320</v>
       </c>
@@ -12114,7 +12116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="217" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="10" t="s">
         <v>321</v>
       </c>
@@ -12148,7 +12150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="10" t="s">
         <v>322</v>
       </c>
@@ -12184,7 +12186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A219" s="10" t="s">
         <v>324</v>
       </c>
@@ -12238,7 +12240,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A220" s="25" t="s">
         <v>329</v>
       </c>
@@ -12278,7 +12280,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:21" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="25" t="s">
         <v>334</v>
       </c>
@@ -12318,7 +12320,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A222" s="25" t="s">
         <v>333</v>
       </c>
@@ -12358,7 +12360,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:21" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:21" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="25" t="s">
         <v>335</v>
       </c>
@@ -12396,7 +12398,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A224" s="25" t="s">
         <v>338</v>
       </c>
@@ -12436,7 +12438,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A225" s="10" t="s">
         <v>339</v>
       </c>
@@ -12472,7 +12474,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A226" s="25" t="s">
         <v>342</v>
       </c>
@@ -12510,7 +12512,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A227" s="25" t="s">
         <v>343</v>
       </c>
@@ -12550,7 +12552,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A228" s="25" t="s">
         <v>344</v>
       </c>
@@ -12588,7 +12590,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A229" s="10" t="s">
         <v>345</v>
       </c>
@@ -12626,7 +12628,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A230" s="10" t="s">
         <v>347</v>
       </c>
@@ -12666,7 +12668,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A231" s="25" t="s">
         <v>349</v>
       </c>
@@ -12706,7 +12708,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A232" s="38" t="s">
         <v>350</v>
       </c>
@@ -12744,7 +12746,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A233" s="10" t="s">
         <v>353</v>
       </c>
@@ -12782,7 +12784,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A234" s="10" t="s">
         <v>354</v>
       </c>
@@ -12820,7 +12822,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="235" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A235" s="10" t="s">
         <v>356</v>
       </c>
@@ -12858,7 +12860,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="236" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A236" s="10" t="s">
         <v>358</v>
       </c>
@@ -12894,7 +12896,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A237" s="10" t="s">
         <v>359</v>
       </c>
@@ -12932,7 +12934,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A238" s="10" t="s">
         <v>361</v>
       </c>
@@ -12972,7 +12974,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A239" s="38" t="s">
         <v>365</v>
       </c>
@@ -13012,7 +13014,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A240" s="25" t="s">
         <v>366</v>
       </c>
@@ -13052,7 +13054,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A241" s="25" t="s">
         <v>367</v>
       </c>
@@ -13090,7 +13092,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A242" s="25" t="s">
         <v>370</v>
       </c>
@@ -13130,7 +13132,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A243" s="25" t="s">
         <v>371</v>
       </c>
@@ -13170,7 +13172,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A244" s="25" t="s">
         <v>372</v>
       </c>
@@ -13210,7 +13212,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A245" s="25" t="s">
         <v>373</v>
       </c>
@@ -13244,7 +13246,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="25" t="s">
         <v>796</v>
       </c>
@@ -13278,7 +13280,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A247" s="10" t="s">
         <v>374</v>
       </c>
@@ -13316,7 +13318,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A248" s="10" t="s">
         <v>375</v>
       </c>
@@ -13350,7 +13352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A249" s="10" t="s">
         <v>376</v>
       </c>
@@ -13384,7 +13386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A250" s="10" t="s">
         <v>377</v>
       </c>
@@ -13422,7 +13424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="251" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A251" s="10" t="s">
         <v>378</v>
       </c>
@@ -13456,7 +13458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A252" s="10" t="s">
         <v>379</v>
       </c>
@@ -13492,7 +13494,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="253" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A253" s="10" t="s">
         <v>381</v>
       </c>
@@ -13526,7 +13528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A254" s="10" t="s">
         <v>382</v>
       </c>
@@ -13558,7 +13560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A255" s="10" t="s">
         <v>383</v>
       </c>
@@ -13600,7 +13602,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="256" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A256" s="10" t="s">
         <v>385</v>
       </c>
@@ -13650,7 +13652,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="257" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A257" s="10" t="s">
         <v>386</v>
       </c>
@@ -13702,7 +13704,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="258" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A258" s="10" t="s">
         <v>387</v>
       </c>
@@ -13756,7 +13758,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A259" s="10" t="s">
         <v>388</v>
       </c>
@@ -13790,7 +13792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A260" s="10" t="s">
         <v>389</v>
       </c>
@@ -13824,7 +13826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A261" s="25" t="s">
         <v>390</v>
       </c>
@@ -13860,7 +13862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A262" s="25" t="s">
         <v>393</v>
       </c>
@@ -13896,7 +13898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A263" s="25" t="s">
         <v>395</v>
       </c>
@@ -13934,7 +13936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A264" s="25" t="s">
         <v>396</v>
       </c>
@@ -13972,7 +13974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A265" s="38" t="s">
         <v>397</v>
       </c>
@@ -14010,7 +14012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A266" s="38" t="s">
         <v>398</v>
       </c>
@@ -14046,7 +14048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A267" s="10" t="s">
         <v>391</v>
       </c>
@@ -14080,7 +14082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A268" s="10" t="s">
         <v>400</v>
       </c>
@@ -14116,7 +14118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A269" s="25" t="s">
         <v>402</v>
       </c>
@@ -14154,7 +14156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A270" s="25" t="s">
         <v>403</v>
       </c>
@@ -14190,7 +14192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A271" s="25" t="s">
         <v>404</v>
       </c>
@@ -14226,7 +14228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A272" s="25" t="s">
         <v>405</v>
       </c>
@@ -14262,7 +14264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A273" s="10" t="s">
         <v>406</v>
       </c>
@@ -14298,7 +14300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A274" s="10" t="s">
         <v>407</v>
       </c>
@@ -14334,7 +14336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A275" s="10" t="s">
         <v>408</v>
       </c>
@@ -14374,7 +14376,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A276" s="10" t="s">
         <v>409</v>
       </c>
@@ -14410,7 +14412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A277" s="10" t="s">
         <v>410</v>
       </c>
@@ -14446,7 +14448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A278" s="25" t="s">
         <v>413</v>
       </c>
@@ -14484,7 +14486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A279" s="25" t="s">
         <v>415</v>
       </c>
@@ -14520,7 +14522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A280" s="25" t="s">
         <v>416</v>
       </c>
@@ -14556,7 +14558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A281" s="25" t="s">
         <v>418</v>
       </c>
@@ -14594,7 +14596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A282" s="25" t="s">
         <v>419</v>
       </c>
@@ -14630,7 +14632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A283" s="25" t="s">
         <v>420</v>
       </c>
@@ -14666,7 +14668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A284" s="25" t="s">
         <v>421</v>
       </c>
@@ -14704,7 +14706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A285" s="10" t="s">
         <v>423</v>
       </c>
@@ -14740,7 +14742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A286" s="10" t="s">
         <v>426</v>
       </c>
@@ -14776,7 +14778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A287" s="10" t="s">
         <v>428</v>
       </c>
@@ -14812,7 +14814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A288" s="10" t="s">
         <v>429</v>
       </c>
@@ -14848,7 +14850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A289" s="10" t="s">
         <v>431</v>
       </c>
@@ -14884,7 +14886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A290" s="10" t="s">
         <v>433</v>
       </c>
@@ -14928,7 +14930,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="291" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A291" s="10" t="s">
         <v>434</v>
       </c>
@@ -14964,7 +14966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A292" s="10" t="s">
         <v>424</v>
       </c>
@@ -15000,7 +15002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A293" s="10" t="s">
         <v>436</v>
       </c>
@@ -15036,7 +15038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A294" s="10" t="s">
         <v>438</v>
       </c>
@@ -15072,7 +15074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A295" s="10" t="s">
         <v>439</v>
       </c>
@@ -15108,7 +15110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A296" s="10" t="s">
         <v>441</v>
       </c>
@@ -15144,7 +15146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A297" s="10" t="s">
         <v>442</v>
       </c>
@@ -15180,7 +15182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A298" s="10" t="s">
         <v>443</v>
       </c>
@@ -15232,7 +15234,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="299" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A299" s="10" t="s">
         <v>445</v>
       </c>
@@ -15264,7 +15266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:22" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A300" s="10" t="s">
         <v>446</v>
       </c>
@@ -15312,7 +15314,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="301" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A301" s="10" t="s">
         <v>447</v>
       </c>
@@ -15361,7 +15363,7 @@
       </c>
       <c r="V301" s="46"/>
     </row>
-    <row r="302" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A302" s="10" t="s">
         <v>448</v>
       </c>
@@ -15403,7 +15405,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="303" spans="1:22" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A303" s="10" t="s">
         <v>449</v>
       </c>
@@ -15453,7 +15455,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="304" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A304" s="10" t="s">
         <v>450</v>
       </c>
@@ -15489,7 +15491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A305" s="10" t="s">
         <v>452</v>
       </c>
@@ -15535,7 +15537,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A306" s="10" t="s">
         <v>453</v>
       </c>
@@ -15579,7 +15581,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="307" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A307" s="10" t="s">
         <v>454</v>
       </c>
@@ -15631,7 +15633,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="308" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A308" s="10" t="s">
         <v>455</v>
       </c>
@@ -15683,7 +15685,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="309" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A309" s="10" t="s">
         <v>457</v>
       </c>
@@ -15717,7 +15719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A310" s="10" t="s">
         <v>458</v>
       </c>
@@ -15751,7 +15753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:21" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:21" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A311" s="25" t="s">
         <v>459</v>
       </c>
@@ -15789,7 +15791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:21" ht="66" x14ac:dyDescent="0.25">
       <c r="A312" s="25" t="s">
         <v>462</v>
       </c>
@@ -15827,7 +15829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:21" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A313" s="10" t="s">
         <v>464</v>
       </c>
@@ -15869,7 +15871,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="314" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:21" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A314" s="10" t="s">
         <v>466</v>
       </c>
@@ -15907,7 +15909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:21" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:21" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" s="10" t="s">
         <v>460</v>
       </c>
@@ -15943,7 +15945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:21" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A316" s="10" t="s">
         <v>468</v>
       </c>
@@ -15981,7 +15983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:21" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A317" s="10" t="s">
         <v>469</v>
       </c>
@@ -16017,7 +16019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="10" t="s">
         <v>471</v>
       </c>
@@ -16051,7 +16053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A319" s="10" t="s">
         <v>474</v>
       </c>
@@ -16087,7 +16089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:21" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A320" s="10" t="s">
         <v>476</v>
       </c>
@@ -16125,7 +16127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:21" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A321" s="10" t="s">
         <v>478</v>
       </c>
@@ -16163,7 +16165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A322" s="10" t="s">
         <v>480</v>
       </c>
@@ -16199,7 +16201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A323" s="10" t="s">
         <v>482</v>
       </c>
@@ -16235,7 +16237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A324" s="10" t="s">
         <v>484</v>
       </c>
@@ -16269,7 +16271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A325" s="10" t="s">
         <v>485</v>
       </c>
@@ -16301,7 +16303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A326" s="10" t="s">
         <v>488</v>
       </c>
@@ -16335,7 +16337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A327" s="10" t="s">
         <v>489</v>
       </c>
@@ -16375,7 +16377,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="328" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A328" s="10" t="s">
         <v>490</v>
       </c>
@@ -16411,7 +16413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A329" s="10" t="s">
         <v>492</v>
       </c>
@@ -16445,7 +16447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A330" s="10" t="s">
         <v>493</v>
       </c>
@@ -16497,7 +16499,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="331" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A331" s="10" t="s">
         <v>494</v>
       </c>
@@ -16543,7 +16545,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="332" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A332" s="10" t="s">
         <v>495</v>
       </c>
@@ -16587,7 +16589,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="333" spans="1:21" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:21" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="10" t="s">
         <v>496</v>
       </c>
@@ -16631,7 +16633,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="334" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A334" s="10" t="s">
         <v>498</v>
       </c>
@@ -16665,7 +16667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A335" s="10" t="s">
         <v>499</v>
       </c>
@@ -16697,7 +16699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A336" s="10" t="s">
         <v>501</v>
       </c>
@@ -16733,7 +16735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A337" s="10" t="s">
         <v>503</v>
       </c>
@@ -16769,7 +16771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A338" s="10" t="s">
         <v>505</v>
       </c>
@@ -16805,7 +16807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A339" s="10" t="s">
         <v>507</v>
       </c>
@@ -16841,7 +16843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A340" s="10" t="s">
         <v>509</v>
       </c>
@@ -16877,7 +16879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A341" s="10" t="s">
         <v>510</v>
       </c>
@@ -16913,7 +16915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A342" s="10" t="s">
         <v>512</v>
       </c>
@@ -16946,7 +16948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A343" s="57" t="s">
         <v>858</v>
       </c>
@@ -16978,7 +16980,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="344" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A344" s="10" t="s">
         <v>513</v>
       </c>
@@ -17010,7 +17012,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="345" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A345" s="10" t="s">
         <v>515</v>
       </c>
@@ -17042,7 +17044,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="346" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A346" s="10" t="s">
         <v>516</v>
       </c>
@@ -17074,7 +17076,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="347" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A347" s="10" t="s">
         <v>517</v>
       </c>
@@ -17106,7 +17108,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="348" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A348" s="10" t="s">
         <v>518</v>
       </c>
@@ -17138,7 +17140,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="349" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A349" s="10" t="s">
         <v>519</v>
       </c>
@@ -17170,7 +17172,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="350" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A350" s="10" t="s">
         <v>520</v>
       </c>
@@ -17202,7 +17204,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="351" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A351" s="10" t="s">
         <v>521</v>
       </c>
@@ -17236,7 +17238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A352" s="10" t="s">
         <v>523</v>
       </c>
@@ -17272,7 +17274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A353" s="10" t="s">
         <v>525</v>
       </c>
@@ -17308,7 +17310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A354" s="10" t="s">
         <v>527</v>
       </c>
@@ -17344,7 +17346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A355" s="10" t="s">
         <v>528</v>
       </c>
@@ -17378,7 +17380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A356" s="10" t="s">
         <v>530</v>
       </c>
@@ -17414,7 +17416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A357" s="10" t="s">
         <v>532</v>
       </c>
@@ -17446,7 +17448,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="358" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A358" s="10" t="s">
         <v>841</v>
       </c>
@@ -17478,7 +17480,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="359" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A359" s="10" t="s">
         <v>533</v>
       </c>
@@ -17510,7 +17512,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="360" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A360" s="10" t="s">
         <v>534</v>
       </c>
@@ -17546,7 +17548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A361" s="25" t="s">
         <v>535</v>
       </c>
@@ -17582,7 +17584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A362" s="25" t="s">
         <v>537</v>
       </c>
@@ -17614,7 +17616,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="363" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A363" s="10" t="s">
         <v>538</v>
       </c>
@@ -17650,7 +17652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A364" s="10" t="s">
         <v>539</v>
       </c>
@@ -17686,7 +17688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A365" s="10" t="s">
         <v>541</v>
       </c>
@@ -17722,7 +17724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A366" s="10" t="s">
         <v>542</v>
       </c>
@@ -17756,7 +17758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A367" s="10" t="s">
         <v>545</v>
       </c>
@@ -17792,7 +17794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A368" s="10" t="s">
         <v>607</v>
       </c>
@@ -17824,7 +17826,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="369" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A369" s="25" t="s">
         <v>547</v>
       </c>
@@ -17860,7 +17862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A370" s="10" t="s">
         <v>548</v>
       </c>
@@ -17896,7 +17898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A371" s="10" t="s">
         <v>549</v>
       </c>
@@ -17934,7 +17936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A372" s="10" t="s">
         <v>551</v>
       </c>
@@ -17970,7 +17972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A373" s="10" t="s">
         <v>553</v>
       </c>
@@ -18000,7 +18002,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="374" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A374" s="10" t="s">
         <v>555</v>
       </c>
@@ -18032,7 +18034,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="375" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A375" s="10" t="s">
         <v>556</v>
       </c>
@@ -18068,7 +18070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A376" s="10" t="s">
         <v>557</v>
       </c>
@@ -18104,7 +18106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A377" s="10" t="s">
         <v>558</v>
       </c>
@@ -18134,7 +18136,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="378" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A378" s="10" t="s">
         <v>560</v>
       </c>
@@ -18166,7 +18168,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="379" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A379" s="10" t="s">
         <v>790</v>
       </c>
@@ -18198,7 +18200,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="380" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A380" s="10" t="s">
         <v>561</v>
       </c>
@@ -18230,7 +18232,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="381" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A381" s="10" t="s">
         <v>562</v>
       </c>
@@ -18266,7 +18268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A382" s="25" t="s">
         <v>564</v>
       </c>
@@ -18302,7 +18304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A383" s="10" t="s">
         <v>565</v>
       </c>
@@ -18336,7 +18338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A384" s="10" t="s">
         <v>566</v>
       </c>
@@ -18370,7 +18372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A385" s="10" t="s">
         <v>567</v>
       </c>
@@ -18404,7 +18406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A386" s="10" t="s">
         <v>569</v>
       </c>
@@ -18442,7 +18444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A387" s="10" t="s">
         <v>572</v>
       </c>
@@ -18476,7 +18478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A388" s="10" t="s">
         <v>574</v>
       </c>
@@ -18512,7 +18514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A389" s="10" t="s">
         <v>576</v>
       </c>
@@ -18548,7 +18550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A390" s="10" t="s">
         <v>577</v>
       </c>
@@ -18584,7 +18586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A391" s="10" t="s">
         <v>578</v>
       </c>
@@ -18620,7 +18622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A392" s="10" t="s">
         <v>579</v>
       </c>
@@ -18656,7 +18658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A393" s="10" t="s">
         <v>580</v>
       </c>
@@ -18692,7 +18694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A394" s="10" t="s">
         <v>581</v>
       </c>
@@ -18726,7 +18728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A395" s="10" t="s">
         <v>583</v>
       </c>
@@ -18762,7 +18764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A396" s="10" t="s">
         <v>585</v>
       </c>
@@ -18798,7 +18800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A397" s="10" t="s">
         <v>793</v>
       </c>
@@ -18830,7 +18832,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="398" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A398" s="10" t="s">
         <v>587</v>
       </c>
@@ -18866,7 +18868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A399" s="10" t="s">
         <v>588</v>
       </c>
@@ -18902,7 +18904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:21" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:21" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="10" t="s">
         <v>589</v>
       </c>
@@ -18940,7 +18942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A401" s="10" t="s">
         <v>592</v>
       </c>
@@ -18976,7 +18978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:21" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:21" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A402" s="10" t="s">
         <v>593</v>
       </c>
@@ -19014,7 +19016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A403" s="10" t="s">
         <v>595</v>
       </c>
@@ -19050,7 +19052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A404" s="10" t="s">
         <v>597</v>
       </c>
@@ -19084,7 +19086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A405" s="10" t="s">
         <v>599</v>
       </c>
@@ -19120,7 +19122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A406" s="10" t="s">
         <v>601</v>
       </c>
@@ -19156,7 +19158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A407" s="10" t="s">
         <v>602</v>
       </c>
@@ -19192,7 +19194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A408" s="10" t="s">
         <v>603</v>
       </c>
@@ -19230,7 +19232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A409" s="10" t="s">
         <v>605</v>
       </c>
@@ -19268,7 +19270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A410" s="10" t="s">
         <v>606</v>
       </c>
@@ -19304,7 +19306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A411" s="10" t="s">
         <v>610</v>
       </c>
@@ -19340,7 +19342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A412" s="10" t="s">
         <v>612</v>
       </c>
@@ -19376,7 +19378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A413" s="10" t="s">
         <v>613</v>
       </c>
@@ -19412,7 +19414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:21" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A414" s="10" t="s">
         <v>614</v>
       </c>
@@ -19450,7 +19452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A415" s="10" t="s">
         <v>616</v>
       </c>
@@ -19484,7 +19486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:21" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:21" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A416" s="10" t="s">
         <v>611</v>
       </c>
@@ -19522,7 +19524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A417" s="10" t="s">
         <v>618</v>
       </c>
@@ -19558,7 +19560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A418" s="10" t="s">
         <v>621</v>
       </c>
@@ -19594,7 +19596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A419" s="10" t="s">
         <v>622</v>
       </c>
@@ -19630,7 +19632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:21" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:21" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A420" s="10" t="s">
         <v>623</v>
       </c>
@@ -19666,7 +19668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A421" s="10" t="s">
         <v>625</v>
       </c>
@@ -19700,7 +19702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A422" s="10" t="s">
         <v>627</v>
       </c>
@@ -19736,7 +19738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A423" s="10" t="s">
         <v>629</v>
       </c>
@@ -19770,7 +19772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A424" s="10" t="s">
         <v>630</v>
       </c>
@@ -19816,7 +19818,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="425" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A425" s="10" t="s">
         <v>632</v>
       </c>
@@ -19850,7 +19852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A426" s="10" t="s">
         <v>633</v>
       </c>
@@ -19888,7 +19890,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="427" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A427" s="10" t="s">
         <v>635</v>
       </c>
@@ -19940,7 +19942,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="428" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A428" s="10" t="s">
         <v>636</v>
       </c>
@@ -19974,7 +19976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A429" s="10" t="s">
         <v>637</v>
       </c>
@@ -20008,7 +20010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A430" s="10" t="s">
         <v>638</v>
       </c>
@@ -20040,7 +20042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A431" s="10" t="s">
         <v>639</v>
       </c>
@@ -20068,7 +20070,7 @@
       </c>
       <c r="R431" s="13"/>
     </row>
-    <row r="432" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A432" s="10" t="s">
         <v>642</v>
       </c>
@@ -20096,7 +20098,7 @@
       </c>
       <c r="R432" s="13"/>
     </row>
-    <row r="433" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A433" s="10" t="s">
         <v>644</v>
       </c>
@@ -20122,7 +20124,7 @@
       </c>
       <c r="R433" s="13"/>
     </row>
-    <row r="434" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A434" s="10" t="s">
         <v>645</v>
       </c>
@@ -20148,7 +20150,7 @@
       </c>
       <c r="R434" s="13"/>
     </row>
-    <row r="435" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A435" s="25" t="s">
         <v>646</v>
       </c>
@@ -20184,7 +20186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A436" s="10" t="s">
         <v>649</v>
       </c>
@@ -20222,7 +20224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="437" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A437" s="10" t="s">
         <v>653</v>
       </c>
@@ -20260,7 +20262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A438" s="10" t="s">
         <v>656</v>
       </c>
@@ -20308,7 +20310,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="439" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A439" s="10" t="s">
         <v>658</v>
       </c>
@@ -20346,7 +20348,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="440" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A440" s="10" t="s">
         <v>661</v>
       </c>
@@ -20384,7 +20386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A441" s="10" t="s">
         <v>664</v>
       </c>
@@ -20420,7 +20422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A442" s="10" t="s">
         <v>667</v>
       </c>
@@ -20456,7 +20458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A443" s="10" t="s">
         <v>669</v>
       </c>
@@ -20502,7 +20504,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="444" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A444" s="10" t="s">
         <v>671</v>
       </c>
@@ -20538,7 +20540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A445" s="10" t="s">
         <v>674</v>
       </c>
@@ -20574,7 +20576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A446" s="10" t="s">
         <v>670</v>
       </c>
@@ -20608,7 +20610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A447" s="10" t="s">
         <v>675</v>
       </c>
@@ -20642,7 +20644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A448" s="10" t="s">
         <v>676</v>
       </c>
@@ -20676,7 +20678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A449" s="10" t="s">
         <v>678</v>
       </c>
@@ -20720,7 +20722,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="450" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A450" s="10" t="s">
         <v>679</v>
       </c>
@@ -20756,7 +20758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A451" s="10" t="s">
         <v>680</v>
       </c>
@@ -20792,7 +20794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A452" s="10" t="s">
         <v>682</v>
       </c>
@@ -20826,7 +20828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A453" s="10" t="s">
         <v>684</v>
       </c>
@@ -20862,7 +20864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A454" s="25" t="s">
         <v>685</v>
       </c>
@@ -20898,7 +20900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A455" s="25" t="s">
         <v>687</v>
       </c>
@@ -20934,7 +20936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A456" s="10" t="s">
         <v>689</v>
       </c>
@@ -20988,7 +20990,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="457" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A457" s="10" t="s">
         <v>690</v>
       </c>
@@ -21022,7 +21024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:21" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A458" s="10" t="s">
         <v>691</v>
       </c>
@@ -21076,7 +21078,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="459" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A459" s="10" t="s">
         <v>692</v>
       </c>
@@ -21122,7 +21124,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="460" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A460" s="10" t="s">
         <v>693</v>
       </c>
@@ -21176,7 +21178,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="461" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A461" s="10" t="s">
         <v>694</v>
       </c>
@@ -21210,7 +21212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:21" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:21" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A462" s="10" t="s">
         <v>695</v>
       </c>
@@ -21260,7 +21262,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="463" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A463" s="10" t="s">
         <v>696</v>
       </c>
@@ -21296,7 +21298,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="464" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A464" s="10" t="s">
         <v>697</v>
       </c>
@@ -21330,7 +21332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A465" s="10" t="s">
         <v>698</v>
       </c>
@@ -21380,7 +21382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="466" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A466" s="10" t="s">
         <v>699</v>
       </c>
@@ -21414,7 +21416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:21" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A467" s="10" t="s">
         <v>700</v>
       </c>
@@ -21468,7 +21470,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="468" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A468" s="10" t="s">
         <v>702</v>
       </c>
@@ -21508,7 +21510,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="469" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A469" s="10" t="s">
         <v>704</v>
       </c>
@@ -21546,7 +21548,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="470" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A470" s="10" t="s">
         <v>707</v>
       </c>
@@ -21580,7 +21582,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="471" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A471" s="27" t="s">
         <v>708</v>
       </c>
@@ -21618,7 +21620,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="472" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A472" s="10" t="s">
         <v>709</v>
       </c>
@@ -21666,7 +21668,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="473" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A473" s="36" t="s">
         <v>710</v>
       </c>
@@ -21700,7 +21702,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="474" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A474" s="38" t="s">
         <v>326</v>
       </c>
@@ -21736,7 +21738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A475" s="25" t="s">
         <v>330</v>
       </c>
@@ -21770,7 +21772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="476" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A476" s="10" t="s">
         <v>337</v>
       </c>
@@ -21804,7 +21806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A477" s="10" t="s">
         <v>340</v>
       </c>
@@ -21838,7 +21840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="478" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A478" s="25" t="s">
         <v>341</v>
       </c>
@@ -21872,7 +21874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A479" s="38" t="s">
         <v>733</v>
       </c>
@@ -21906,7 +21908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:21" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A480" s="10" t="s">
         <v>362</v>
       </c>
@@ -21940,7 +21942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A481" s="10" t="s">
         <v>713</v>
       </c>
@@ -21964,7 +21966,7 @@
       </c>
       <c r="R481" s="13"/>
     </row>
-    <row r="482" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A482" s="10" t="s">
         <v>714</v>
       </c>
@@ -21988,7 +21990,7 @@
       </c>
       <c r="R482" s="13"/>
     </row>
-    <row r="483" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A483" s="10" t="s">
         <v>715</v>
       </c>
@@ -22012,7 +22014,7 @@
       </c>
       <c r="R483" s="13"/>
     </row>
-    <row r="484" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A484" s="10" t="s">
         <v>716</v>
       </c>
@@ -22036,7 +22038,7 @@
       </c>
       <c r="R484" s="13"/>
     </row>
-    <row r="485" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A485" s="10" t="s">
         <v>717</v>
       </c>
@@ -22060,7 +22062,7 @@
       </c>
       <c r="R485" s="13"/>
     </row>
-    <row r="486" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A486" s="10" t="s">
         <v>718</v>
       </c>
@@ -22084,7 +22086,7 @@
       </c>
       <c r="R486" s="13"/>
     </row>
-    <row r="487" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A487" s="10" t="s">
         <v>719</v>
       </c>
@@ -22108,7 +22110,7 @@
       </c>
       <c r="R487" s="13"/>
     </row>
-    <row r="488" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A488" s="10" t="s">
         <v>720</v>
       </c>
@@ -22132,7 +22134,7 @@
       </c>
       <c r="R488" s="13"/>
     </row>
-    <row r="489" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A489" s="10" t="s">
         <v>721</v>
       </c>
@@ -22156,7 +22158,7 @@
       </c>
       <c r="R489" s="13"/>
     </row>
-    <row r="490" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A490" s="10" t="s">
         <v>722</v>
       </c>
@@ -22180,7 +22182,7 @@
       </c>
       <c r="R490" s="13"/>
     </row>
-    <row r="491" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A491" s="10" t="s">
         <v>723</v>
       </c>
@@ -22204,7 +22206,7 @@
       </c>
       <c r="R491" s="13"/>
     </row>
-    <row r="492" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A492" s="10" t="s">
         <v>724</v>
       </c>
@@ -22228,7 +22230,7 @@
       </c>
       <c r="R492" s="13"/>
     </row>
-    <row r="493" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A493" s="10" t="s">
         <v>725</v>
       </c>
@@ -22252,7 +22254,7 @@
       </c>
       <c r="R493" s="13"/>
     </row>
-    <row r="494" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A494" s="10" t="s">
         <v>726</v>
       </c>
@@ -22276,7 +22278,7 @@
       </c>
       <c r="R494" s="13"/>
     </row>
-    <row r="495" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A495" s="10" t="s">
         <v>727</v>
       </c>
@@ -22300,7 +22302,7 @@
       </c>
       <c r="R495" s="13"/>
     </row>
-    <row r="496" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A496" s="10" t="s">
         <v>728</v>
       </c>
@@ -22324,7 +22326,7 @@
       </c>
       <c r="R496" s="13"/>
     </row>
-    <row r="497" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A497" s="10" t="s">
         <v>729</v>
       </c>
@@ -22348,7 +22350,7 @@
       </c>
       <c r="R497" s="13"/>
     </row>
-    <row r="498" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A498" s="10" t="s">
         <v>731</v>
       </c>
@@ -22372,7 +22374,7 @@
       </c>
       <c r="R498" s="13"/>
     </row>
-    <row r="499" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q499" s="34"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added urban/rural to alt receps
</commit_message>
<xml_diff>
--- a/resources/Dose_Response_Library.xlsx
+++ b/resources/Dose_Response_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_HEM4\HEM4\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scainccloud-my.sharepoint.com/personal/jmozier_scainc_com/Documents/Projects/ASRA-RIS-BasePeriod/HEM4_HEM5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296BCBA1-A4F7-40D2-98F8-5061F720BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C8A4702-D671-4436-86AA-93B15A43F381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="16320" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dose Response Value Library" sheetId="1" r:id="rId1"/>
@@ -2965,22 +2965,22 @@
       <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.77734375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
     <col min="3" max="3" width="14" style="26" customWidth="1"/>
     <col min="4" max="4" width="21" style="6" customWidth="1"/>
     <col min="5" max="5" width="11" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" style="27" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" style="27" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="27" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" style="27" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="27" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="27" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="27" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="27" customWidth="1"/>
     <col min="10" max="10" width="12" style="27" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="6"/>
+    <col min="11" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="48.3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="48.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -3064,7 +3064,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -3084,7 +3084,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -3128,7 +3128,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -3148,7 +3148,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -3168,7 +3168,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -3190,7 +3190,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -3212,7 +3212,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -3234,7 +3234,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -3256,7 +3256,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
@@ -3282,7 +3282,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
@@ -3358,7 +3358,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
@@ -3380,7 +3380,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
@@ -3402,7 +3402,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>28</v>
       </c>
@@ -3424,7 +3424,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
@@ -3470,7 +3470,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>32</v>
       </c>
@@ -3492,7 +3492,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
@@ -3514,7 +3514,7 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
@@ -3536,7 +3536,7 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
@@ -3558,7 +3558,7 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
@@ -3578,7 +3578,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
@@ -3598,7 +3598,7 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>39</v>
       </c>
@@ -3620,7 +3620,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>40</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>41</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
@@ -3704,7 +3704,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>43</v>
       </c>
@@ -3726,7 +3726,7 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>44</v>
       </c>
@@ -3748,7 +3748,7 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>45</v>
       </c>
@@ -3768,7 +3768,7 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>46</v>
       </c>
@@ -3788,7 +3788,7 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>47</v>
       </c>
@@ -3810,7 +3810,7 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>48</v>
       </c>
@@ -3832,7 +3832,7 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>49</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>51</v>
       </c>
@@ -3880,7 +3880,7 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>53</v>
       </c>
@@ -3898,7 +3898,7 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>54</v>
       </c>
@@ -3916,7 +3916,7 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
@@ -3938,7 +3938,7 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>56</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>57</v>
       </c>
@@ -3992,7 +3992,7 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>58</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>59</v>
       </c>
@@ -4040,7 +4040,7 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>60</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>61</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>62</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>63</v>
       </c>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>64</v>
       </c>
@@ -4184,7 +4184,7 @@
       </c>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>65</v>
       </c>
@@ -4210,7 +4210,7 @@
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>66</v>
       </c>
@@ -4232,7 +4232,7 @@
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>67</v>
       </c>
@@ -4254,7 +4254,7 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>68</v>
       </c>
@@ -4274,7 +4274,7 @@
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>69</v>
       </c>
@@ -4294,7 +4294,7 @@
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>71</v>
       </c>
@@ -4316,7 +4316,7 @@
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>72</v>
       </c>
@@ -4338,7 +4338,7 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>73</v>
       </c>
@@ -4360,7 +4360,7 @@
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>74</v>
       </c>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>76</v>
       </c>
@@ -4406,7 +4406,7 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>77</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>79</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>80</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
         <v>82</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>84</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>86</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>87</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>88</v>
       </c>
@@ -4610,7 +4610,7 @@
       </c>
       <c r="J69" s="4"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>89</v>
       </c>
@@ -4630,7 +4630,7 @@
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>90</v>
       </c>
@@ -4650,7 +4650,7 @@
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>91</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>92</v>
       </c>
@@ -4700,7 +4700,7 @@
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>93</v>
       </c>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>95</v>
       </c>
@@ -4746,7 +4746,7 @@
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>97</v>
       </c>
@@ -4768,7 +4768,7 @@
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>99</v>
       </c>
@@ -4790,7 +4790,7 @@
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>101</v>
       </c>
@@ -4808,7 +4808,7 @@
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>102</v>
       </c>
@@ -4832,7 +4832,7 @@
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>103</v>
       </c>
@@ -4852,7 +4852,7 @@
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>104</v>
       </c>
@@ -4878,7 +4878,7 @@
       </c>
       <c r="J81" s="4"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>105</v>
       </c>
@@ -4900,7 +4900,7 @@
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
         <v>106</v>
       </c>
@@ -4922,7 +4922,7 @@
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>107</v>
       </c>
@@ -4948,7 +4948,7 @@
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>108</v>
       </c>
@@ -4970,7 +4970,7 @@
       <c r="I85" s="4"/>
       <c r="J85" s="4"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>110</v>
       </c>
@@ -4992,7 +4992,7 @@
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>111</v>
       </c>
@@ -5014,7 +5014,7 @@
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>112</v>
       </c>
@@ -5036,7 +5036,7 @@
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>114</v>
       </c>
@@ -5056,7 +5056,7 @@
       <c r="I89" s="4"/>
       <c r="J89" s="4"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>115</v>
       </c>
@@ -5078,7 +5078,7 @@
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>116</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>117</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>118</v>
       </c>
@@ -5162,7 +5162,7 @@
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>120</v>
       </c>
@@ -5180,7 +5180,7 @@
       <c r="I94" s="4"/>
       <c r="J94" s="4"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>121</v>
       </c>
@@ -5202,7 +5202,7 @@
       <c r="I95" s="4"/>
       <c r="J95" s="4"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>122</v>
       </c>
@@ -5224,7 +5224,7 @@
       <c r="I96" s="4"/>
       <c r="J96" s="4"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>123</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>124</v>
       </c>
@@ -5280,7 +5280,7 @@
       <c r="I98" s="4"/>
       <c r="J98" s="4"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>125</v>
       </c>
@@ -5306,7 +5306,7 @@
       <c r="I99" s="4"/>
       <c r="J99" s="4"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>126</v>
       </c>
@@ -5328,7 +5328,7 @@
       <c r="I100" s="4"/>
       <c r="J100" s="4"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>127</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>128</v>
       </c>
@@ -5382,7 +5382,7 @@
       </c>
       <c r="J102" s="4"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>129</v>
       </c>
@@ -5404,7 +5404,7 @@
       <c r="I103" s="4"/>
       <c r="J103" s="4"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>130</v>
       </c>
@@ -5426,7 +5426,7 @@
       <c r="I104" s="4"/>
       <c r="J104" s="4"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
         <v>132</v>
       </c>
@@ -5448,7 +5448,7 @@
       <c r="I105" s="4"/>
       <c r="J105" s="4"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
         <v>133</v>
       </c>
@@ -5470,7 +5470,7 @@
       <c r="I106" s="4"/>
       <c r="J106" s="4"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="18" t="s">
         <v>134</v>
       </c>
@@ -5492,7 +5492,7 @@
       <c r="I107" s="4"/>
       <c r="J107" s="4"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="18" t="s">
         <v>135</v>
       </c>
@@ -5514,7 +5514,7 @@
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>137</v>
       </c>
@@ -5532,7 +5532,7 @@
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>138</v>
       </c>
@@ -5550,7 +5550,7 @@
       <c r="I110" s="4"/>
       <c r="J110" s="4"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>139</v>
       </c>
@@ -5572,7 +5572,7 @@
       <c r="I111" s="4"/>
       <c r="J111" s="4"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>140</v>
       </c>
@@ -5594,7 +5594,7 @@
       <c r="I112" s="4"/>
       <c r="J112" s="4"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
         <v>141</v>
       </c>
@@ -5616,7 +5616,7 @@
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="18" t="s">
         <v>142</v>
       </c>
@@ -5638,7 +5638,7 @@
       <c r="I114" s="4"/>
       <c r="J114" s="4"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>143</v>
       </c>
@@ -5660,7 +5660,7 @@
       <c r="I115" s="4"/>
       <c r="J115" s="4"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>144</v>
       </c>
@@ -5682,7 +5682,7 @@
       <c r="I116" s="4"/>
       <c r="J116" s="4"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>145</v>
       </c>
@@ -5700,7 +5700,7 @@
       <c r="I117" s="4"/>
       <c r="J117" s="4"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>131</v>
       </c>
@@ -5722,7 +5722,7 @@
       <c r="I118" s="4"/>
       <c r="J118" s="4"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>147</v>
       </c>
@@ -5744,7 +5744,7 @@
       <c r="I119" s="4"/>
       <c r="J119" s="4"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>148</v>
       </c>
@@ -5762,7 +5762,7 @@
       <c r="I120" s="4"/>
       <c r="J120" s="4"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>149</v>
       </c>
@@ -5784,7 +5784,7 @@
       <c r="I121" s="4"/>
       <c r="J121" s="4"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>150</v>
       </c>
@@ -5806,7 +5806,7 @@
       <c r="I122" s="4"/>
       <c r="J122" s="4"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
         <v>151</v>
       </c>
@@ -5828,7 +5828,7 @@
       <c r="I123" s="4"/>
       <c r="J123" s="4"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>152</v>
       </c>
@@ -5850,7 +5850,7 @@
       <c r="I124" s="4"/>
       <c r="J124" s="4"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
         <v>153</v>
       </c>
@@ -5872,7 +5872,7 @@
       <c r="I125" s="4"/>
       <c r="J125" s="4"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="18" t="s">
         <v>154</v>
       </c>
@@ -5894,7 +5894,7 @@
       <c r="I126" s="4"/>
       <c r="J126" s="4"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="18" t="s">
         <v>155</v>
       </c>
@@ -5912,7 +5912,7 @@
       <c r="I127" s="4"/>
       <c r="J127" s="4"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
         <v>156</v>
       </c>
@@ -5934,7 +5934,7 @@
       <c r="I128" s="4"/>
       <c r="J128" s="4"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>157</v>
       </c>
@@ -5954,7 +5954,7 @@
       <c r="I129" s="4"/>
       <c r="J129" s="4"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>159</v>
       </c>
@@ -5974,7 +5974,7 @@
       <c r="I130" s="4"/>
       <c r="J130" s="4"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>161</v>
       </c>
@@ -5994,7 +5994,7 @@
       <c r="I131" s="4"/>
       <c r="J131" s="4"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>163</v>
       </c>
@@ -6014,7 +6014,7 @@
       <c r="I132" s="4"/>
       <c r="J132" s="4"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>165</v>
       </c>
@@ -6034,7 +6034,7 @@
       <c r="I133" s="4"/>
       <c r="J133" s="4"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>158</v>
       </c>
@@ -6056,7 +6056,7 @@
       <c r="I134" s="4"/>
       <c r="J134" s="4"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>167</v>
       </c>
@@ -6078,7 +6078,7 @@
       </c>
       <c r="J135" s="4"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>169</v>
       </c>
@@ -6098,7 +6098,7 @@
       <c r="I136" s="4"/>
       <c r="J136" s="4"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>170</v>
       </c>
@@ -6118,7 +6118,7 @@
       <c r="I137" s="4"/>
       <c r="J137" s="4"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>172</v>
       </c>
@@ -6138,7 +6138,7 @@
       <c r="I138" s="4"/>
       <c r="J138" s="4"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>173</v>
       </c>
@@ -6158,7 +6158,7 @@
       <c r="I139" s="4"/>
       <c r="J139" s="4"/>
     </row>
-    <row r="140" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>174</v>
       </c>
@@ -6178,7 +6178,7 @@
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>175</v>
       </c>
@@ -6198,7 +6198,7 @@
       <c r="I141" s="4"/>
       <c r="J141" s="4"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>452</v>
       </c>
@@ -6218,7 +6218,7 @@
       <c r="I142" s="4"/>
       <c r="J142" s="4"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>177</v>
       </c>
@@ -6240,7 +6240,7 @@
       <c r="I143" s="4"/>
       <c r="J143" s="4"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>178</v>
       </c>
@@ -6260,7 +6260,7 @@
       <c r="I144" s="4"/>
       <c r="J144" s="4"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>179</v>
       </c>
@@ -6282,7 +6282,7 @@
       <c r="I145" s="4"/>
       <c r="J145" s="4"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>181</v>
       </c>
@@ -6304,7 +6304,7 @@
       <c r="I146" s="4"/>
       <c r="J146" s="4"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>182</v>
       </c>
@@ -6326,7 +6326,7 @@
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>183</v>
       </c>
@@ -6348,7 +6348,7 @@
       <c r="I148" s="4"/>
       <c r="J148" s="4"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>184</v>
       </c>
@@ -6374,7 +6374,7 @@
       <c r="I149" s="4"/>
       <c r="J149" s="4"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>185</v>
       </c>
@@ -6400,7 +6400,7 @@
       <c r="I150" s="4"/>
       <c r="J150" s="4"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
         <v>187</v>
       </c>
@@ -6420,7 +6420,7 @@
       <c r="I151" s="4"/>
       <c r="J151" s="4"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>189</v>
       </c>
@@ -6440,7 +6440,7 @@
       <c r="I152" s="4"/>
       <c r="J152" s="4"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>191</v>
       </c>
@@ -6466,7 +6466,7 @@
       <c r="I153" s="4"/>
       <c r="J153" s="4"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>192</v>
       </c>
@@ -6488,7 +6488,7 @@
       <c r="I154" s="4"/>
       <c r="J154" s="4"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>193</v>
       </c>
@@ -6508,7 +6508,7 @@
       <c r="I155" s="4"/>
       <c r="J155" s="4"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>194</v>
       </c>
@@ -6528,7 +6528,7 @@
       <c r="I156" s="4"/>
       <c r="J156" s="4"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>186</v>
       </c>
@@ -6550,7 +6550,7 @@
       <c r="I157" s="4"/>
       <c r="J157" s="4"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>195</v>
       </c>
@@ -6576,7 +6576,7 @@
       <c r="I158" s="4"/>
       <c r="J158" s="4"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>196</v>
       </c>
@@ -6598,7 +6598,7 @@
       <c r="I159" s="4"/>
       <c r="J159" s="4"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>197</v>
       </c>
@@ -6622,7 +6622,7 @@
       </c>
       <c r="J160" s="4"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>198</v>
       </c>
@@ -6642,7 +6642,7 @@
       <c r="I161" s="4"/>
       <c r="J161" s="4"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>200</v>
       </c>
@@ -6662,7 +6662,7 @@
       <c r="I162" s="4"/>
       <c r="J162" s="4"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>202</v>
       </c>
@@ -6682,7 +6682,7 @@
       <c r="I163" s="4"/>
       <c r="J163" s="4"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>204</v>
       </c>
@@ -6704,7 +6704,7 @@
       <c r="I164" s="4"/>
       <c r="J164" s="4"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>205</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
         <v>206</v>
       </c>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="J166" s="4"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>207</v>
       </c>
@@ -6786,7 +6786,7 @@
       <c r="I167" s="4"/>
       <c r="J167" s="4"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>208</v>
       </c>
@@ -6808,7 +6808,7 @@
       <c r="I168" s="4"/>
       <c r="J168" s="4"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>209</v>
       </c>
@@ -6828,7 +6828,7 @@
       <c r="I169" s="4"/>
       <c r="J169" s="4"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>211</v>
       </c>
@@ -6850,7 +6850,7 @@
       <c r="I170" s="4"/>
       <c r="J170" s="4"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>212</v>
       </c>
@@ -6876,7 +6876,7 @@
       <c r="I171" s="4"/>
       <c r="J171" s="4"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>213</v>
       </c>
@@ -6898,7 +6898,7 @@
       <c r="I172" s="4"/>
       <c r="J172" s="4"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>215</v>
       </c>
@@ -6920,7 +6920,7 @@
       <c r="I173" s="4"/>
       <c r="J173" s="4"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>216</v>
       </c>
@@ -6942,7 +6942,7 @@
       <c r="I174" s="4"/>
       <c r="J174" s="4"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>217</v>
       </c>
@@ -6962,7 +6962,7 @@
       <c r="I175" s="4"/>
       <c r="J175" s="4"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>219</v>
       </c>
@@ -6980,7 +6980,7 @@
       <c r="I176" s="4"/>
       <c r="J176" s="4"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>221</v>
       </c>
@@ -7002,7 +7002,7 @@
       <c r="I177" s="4"/>
       <c r="J177" s="4"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>222</v>
       </c>
@@ -7024,7 +7024,7 @@
       <c r="I178" s="4"/>
       <c r="J178" s="4"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>223</v>
       </c>
@@ -7046,7 +7046,7 @@
       <c r="I179" s="4"/>
       <c r="J179" s="4"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>224</v>
       </c>
@@ -7070,7 +7070,7 @@
       <c r="I180" s="4"/>
       <c r="J180" s="4"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>225</v>
       </c>
@@ -7092,7 +7092,7 @@
       <c r="I181" s="4"/>
       <c r="J181" s="4"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>227</v>
       </c>
@@ -7114,7 +7114,7 @@
       <c r="I182" s="4"/>
       <c r="J182" s="4"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
         <v>228</v>
       </c>
@@ -7132,7 +7132,7 @@
       <c r="I183" s="4"/>
       <c r="J183" s="4"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>230</v>
       </c>
@@ -7160,7 +7160,7 @@
       </c>
       <c r="J184" s="4"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>231</v>
       </c>
@@ -7182,7 +7182,7 @@
       <c r="I185" s="4"/>
       <c r="J185" s="4"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>232</v>
       </c>
@@ -7208,7 +7208,7 @@
       <c r="I186" s="4"/>
       <c r="J186" s="4"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
         <v>233</v>
       </c>
@@ -7226,7 +7226,7 @@
       <c r="I187" s="4"/>
       <c r="J187" s="4"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>619</v>
       </c>
@@ -7248,7 +7248,7 @@
       <c r="I188" s="4"/>
       <c r="J188" s="4"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>620</v>
       </c>
@@ -7270,7 +7270,7 @@
       <c r="I189" s="4"/>
       <c r="J189" s="4"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>235</v>
       </c>
@@ -7292,7 +7292,7 @@
       <c r="I190" s="4"/>
       <c r="J190" s="4"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
         <v>236</v>
       </c>
@@ -7314,7 +7314,7 @@
       <c r="I191" s="4"/>
       <c r="J191" s="4"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>237</v>
       </c>
@@ -7336,7 +7336,7 @@
       <c r="I192" s="4"/>
       <c r="J192" s="4"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
         <v>238</v>
       </c>
@@ -7358,7 +7358,7 @@
       <c r="I193" s="4"/>
       <c r="J193" s="4"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
         <v>239</v>
       </c>
@@ -7380,7 +7380,7 @@
       <c r="I194" s="4"/>
       <c r="J194" s="4"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
         <v>240</v>
       </c>
@@ -7402,7 +7402,7 @@
       <c r="I195" s="4"/>
       <c r="J195" s="4"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>241</v>
       </c>
@@ -7424,7 +7424,7 @@
       <c r="I196" s="4"/>
       <c r="J196" s="4"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" s="4" t="s">
         <v>242</v>
       </c>
@@ -7446,7 +7446,7 @@
       <c r="I197" s="4"/>
       <c r="J197" s="4"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
         <v>243</v>
       </c>
@@ -7468,7 +7468,7 @@
       <c r="I198" s="4"/>
       <c r="J198" s="4"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
         <v>244</v>
       </c>
@@ -7490,7 +7490,7 @@
       <c r="I199" s="4"/>
       <c r="J199" s="4"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" s="4" t="s">
         <v>245</v>
       </c>
@@ -7512,7 +7512,7 @@
       <c r="I200" s="4"/>
       <c r="J200" s="4"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" s="4" t="s">
         <v>246</v>
       </c>
@@ -7534,7 +7534,7 @@
       <c r="I201" s="4"/>
       <c r="J201" s="4"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
         <v>247</v>
       </c>
@@ -7556,7 +7556,7 @@
       <c r="I202" s="4"/>
       <c r="J202" s="4"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" s="4" t="s">
         <v>248</v>
       </c>
@@ -7578,7 +7578,7 @@
       <c r="I203" s="4"/>
       <c r="J203" s="4"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
         <v>249</v>
       </c>
@@ -7600,7 +7600,7 @@
       <c r="I204" s="4"/>
       <c r="J204" s="4"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
         <v>250</v>
       </c>
@@ -7622,7 +7622,7 @@
       <c r="I205" s="4"/>
       <c r="J205" s="4"/>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
         <v>252</v>
       </c>
@@ -7640,7 +7640,7 @@
       <c r="I206" s="4"/>
       <c r="J206" s="4"/>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" s="4" t="s">
         <v>253</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" s="4" t="s">
         <v>254</v>
       </c>
@@ -7700,7 +7700,7 @@
       </c>
       <c r="J208" s="4"/>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" s="4" t="s">
         <v>255</v>
       </c>
@@ -7726,7 +7726,7 @@
       <c r="I209" s="4"/>
       <c r="J209" s="4"/>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" s="4" t="s">
         <v>256</v>
       </c>
@@ -7748,7 +7748,7 @@
       <c r="I210" s="4"/>
       <c r="J210" s="4"/>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" s="4" t="s">
         <v>257</v>
       </c>
@@ -7770,7 +7770,7 @@
       <c r="I211" s="4"/>
       <c r="J211" s="4"/>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" s="4" t="s">
         <v>258</v>
       </c>
@@ -7796,7 +7796,7 @@
       <c r="I212" s="4"/>
       <c r="J212" s="4"/>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" s="4" t="s">
         <v>259</v>
       </c>
@@ -7822,7 +7822,7 @@
       </c>
       <c r="J213" s="4"/>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
         <v>260</v>
       </c>
@@ -7844,7 +7844,7 @@
       <c r="I214" s="4"/>
       <c r="J214" s="4"/>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" s="4" t="s">
         <v>261</v>
       </c>
@@ -7868,7 +7868,7 @@
       <c r="I215" s="4"/>
       <c r="J215" s="4"/>
     </row>
-    <row r="216" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>262</v>
       </c>
@@ -7894,7 +7894,7 @@
       </c>
       <c r="J216" s="4"/>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" s="4" t="s">
         <v>263</v>
       </c>
@@ -7914,7 +7914,7 @@
       <c r="I217" s="4"/>
       <c r="J217" s="4"/>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" s="4" t="s">
         <v>264</v>
       </c>
@@ -7936,7 +7936,7 @@
       <c r="I218" s="4"/>
       <c r="J218" s="4"/>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" s="4" t="s">
         <v>265</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" s="7" t="s">
         <v>268</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" s="7" t="s">
         <v>272</v>
       </c>
@@ -8016,7 +8016,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" s="7" t="s">
         <v>271</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" s="7" t="s">
         <v>273</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" s="7" t="s">
         <v>275</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" s="4" t="s">
         <v>276</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" s="7" t="s">
         <v>279</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227" s="7" t="s">
         <v>280</v>
       </c>
@@ -8154,7 +8154,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" s="7" t="s">
         <v>281</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" s="4" t="s">
         <v>282</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" s="4" t="s">
         <v>283</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" s="7" t="s">
         <v>284</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" s="18" t="s">
         <v>285</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" s="4" t="s">
         <v>287</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" s="4" t="s">
         <v>288</v>
       </c>
@@ -8316,7 +8316,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" s="4" t="s">
         <v>289</v>
       </c>
@@ -8340,7 +8340,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" s="4" t="s">
         <v>290</v>
       </c>
@@ -8364,7 +8364,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" s="4" t="s">
         <v>291</v>
       </c>
@@ -8388,7 +8388,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" s="4" t="s">
         <v>292</v>
       </c>
@@ -8410,7 +8410,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" s="18" t="s">
         <v>295</v>
       </c>
@@ -8434,7 +8434,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" s="7" t="s">
         <v>296</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" s="7" t="s">
         <v>297</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" s="7" t="s">
         <v>299</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" s="7" t="s">
         <v>300</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244" s="7" t="s">
         <v>301</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245" s="7" t="s">
         <v>302</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" s="7" t="s">
         <v>617</v>
       </c>
@@ -8596,7 +8596,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" s="4" t="s">
         <v>303</v>
       </c>
@@ -8618,7 +8618,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" s="4" t="s">
         <v>304</v>
       </c>
@@ -8640,7 +8640,7 @@
       <c r="I248" s="4"/>
       <c r="J248" s="4"/>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" s="4" t="s">
         <v>305</v>
       </c>
@@ -8660,7 +8660,7 @@
       <c r="I249" s="4"/>
       <c r="J249" s="4"/>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" s="4" t="s">
         <v>306</v>
       </c>
@@ -8684,7 +8684,7 @@
       </c>
       <c r="J250" s="4"/>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" s="4" t="s">
         <v>307</v>
       </c>
@@ -8706,7 +8706,7 @@
       <c r="I251" s="4"/>
       <c r="J251" s="4"/>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" s="4" t="s">
         <v>308</v>
       </c>
@@ -8726,7 +8726,7 @@
       <c r="I252" s="4"/>
       <c r="J252" s="4"/>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" s="4" t="s">
         <v>309</v>
       </c>
@@ -8748,7 +8748,7 @@
       <c r="I253" s="4"/>
       <c r="J253" s="4"/>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" s="4" t="s">
         <v>310</v>
       </c>
@@ -8766,7 +8766,7 @@
       <c r="I254" s="4"/>
       <c r="J254" s="4"/>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" s="4" t="s">
         <v>311</v>
       </c>
@@ -8790,7 +8790,7 @@
       <c r="I255" s="4"/>
       <c r="J255" s="4"/>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" s="4" t="s">
         <v>313</v>
       </c>
@@ -8820,7 +8820,7 @@
       </c>
       <c r="J256" s="4"/>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" s="4" t="s">
         <v>314</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" s="4" t="s">
         <v>315</v>
       </c>
@@ -8884,7 +8884,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" s="4" t="s">
         <v>316</v>
       </c>
@@ -8906,7 +8906,7 @@
       <c r="I259" s="4"/>
       <c r="J259" s="4"/>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" s="4" t="s">
         <v>317</v>
       </c>
@@ -8926,7 +8926,7 @@
       <c r="I260" s="4"/>
       <c r="J260" s="4"/>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" s="7" t="s">
         <v>318</v>
       </c>
@@ -8946,7 +8946,7 @@
       <c r="I261" s="4"/>
       <c r="J261" s="4"/>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" s="7" t="s">
         <v>320</v>
       </c>
@@ -8966,7 +8966,7 @@
       <c r="I262" s="4"/>
       <c r="J262" s="4"/>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" s="7" t="s">
         <v>321</v>
       </c>
@@ -8988,7 +8988,7 @@
       <c r="I263" s="4"/>
       <c r="J263" s="4"/>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" s="7" t="s">
         <v>322</v>
       </c>
@@ -9010,7 +9010,7 @@
       <c r="I264" s="4"/>
       <c r="J264" s="4"/>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" s="18" t="s">
         <v>323</v>
       </c>
@@ -9032,7 +9032,7 @@
       <c r="I265" s="4"/>
       <c r="J265" s="4"/>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" s="18" t="s">
         <v>324</v>
       </c>
@@ -9052,7 +9052,7 @@
       <c r="I266" s="4"/>
       <c r="J266" s="4"/>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" s="4" t="s">
         <v>319</v>
       </c>
@@ -9074,7 +9074,7 @@
       <c r="I267" s="4"/>
       <c r="J267" s="4"/>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268" s="4" t="s">
         <v>326</v>
       </c>
@@ -9094,7 +9094,7 @@
       <c r="I268" s="4"/>
       <c r="J268" s="4"/>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269" s="7" t="s">
         <v>327</v>
       </c>
@@ -9116,7 +9116,7 @@
       <c r="I269" s="4"/>
       <c r="J269" s="4"/>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" s="7" t="s">
         <v>328</v>
       </c>
@@ -9136,7 +9136,7 @@
       <c r="I270" s="4"/>
       <c r="J270" s="4"/>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" s="7" t="s">
         <v>329</v>
       </c>
@@ -9156,7 +9156,7 @@
       <c r="I271" s="4"/>
       <c r="J271" s="4"/>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272" s="7" t="s">
         <v>330</v>
       </c>
@@ -9176,7 +9176,7 @@
       <c r="I272" s="4"/>
       <c r="J272" s="4"/>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" s="4" t="s">
         <v>331</v>
       </c>
@@ -9198,7 +9198,7 @@
       <c r="I273" s="4"/>
       <c r="J273" s="4"/>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" s="4" t="s">
         <v>332</v>
       </c>
@@ -9220,7 +9220,7 @@
       <c r="I274" s="4"/>
       <c r="J274" s="4"/>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275" s="4" t="s">
         <v>333</v>
       </c>
@@ -9246,7 +9246,7 @@
       </c>
       <c r="J275" s="4"/>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" s="4" t="s">
         <v>334</v>
       </c>
@@ -9266,7 +9266,7 @@
       <c r="I276" s="4"/>
       <c r="J276" s="4"/>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" s="4" t="s">
         <v>335</v>
       </c>
@@ -9288,7 +9288,7 @@
       <c r="I277" s="4"/>
       <c r="J277" s="4"/>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" s="7" t="s">
         <v>336</v>
       </c>
@@ -9310,7 +9310,7 @@
       <c r="I278" s="4"/>
       <c r="J278" s="4"/>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279" s="7" t="s">
         <v>337</v>
       </c>
@@ -9330,7 +9330,7 @@
       <c r="I279" s="4"/>
       <c r="J279" s="4"/>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" s="7" t="s">
         <v>338</v>
       </c>
@@ -9350,7 +9350,7 @@
       <c r="I280" s="4"/>
       <c r="J280" s="4"/>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" s="7" t="s">
         <v>340</v>
       </c>
@@ -9372,7 +9372,7 @@
       <c r="I281" s="4"/>
       <c r="J281" s="4"/>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282" s="7" t="s">
         <v>341</v>
       </c>
@@ -9392,7 +9392,7 @@
       <c r="I282" s="4"/>
       <c r="J282" s="4"/>
     </row>
-    <row r="283" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A283" s="7" t="s">
         <v>342</v>
       </c>
@@ -9412,7 +9412,7 @@
       <c r="I283" s="4"/>
       <c r="J283" s="4"/>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284" s="7" t="s">
         <v>343</v>
       </c>
@@ -9434,7 +9434,7 @@
       <c r="I284" s="4"/>
       <c r="J284" s="4"/>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" s="4" t="s">
         <v>344</v>
       </c>
@@ -9454,7 +9454,7 @@
       <c r="I285" s="4"/>
       <c r="J285" s="4"/>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" s="4" t="s">
         <v>346</v>
       </c>
@@ -9474,7 +9474,7 @@
       <c r="I286" s="4"/>
       <c r="J286" s="4"/>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A287" s="4" t="s">
         <v>348</v>
       </c>
@@ -9496,7 +9496,7 @@
       <c r="I287" s="4"/>
       <c r="J287" s="4"/>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288" s="4" t="s">
         <v>349</v>
       </c>
@@ -9516,7 +9516,7 @@
       <c r="I288" s="4"/>
       <c r="J288" s="4"/>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289" s="4" t="s">
         <v>351</v>
       </c>
@@ -9536,7 +9536,7 @@
       <c r="I289" s="4"/>
       <c r="J289" s="4"/>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290" s="4" t="s">
         <v>353</v>
       </c>
@@ -9564,7 +9564,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291" s="4" t="s">
         <v>354</v>
       </c>
@@ -9584,7 +9584,7 @@
       <c r="I291" s="4"/>
       <c r="J291" s="4"/>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292" s="4" t="s">
         <v>345</v>
       </c>
@@ -9606,7 +9606,7 @@
       <c r="I292" s="4"/>
       <c r="J292" s="4"/>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A293" s="4" t="s">
         <v>356</v>
       </c>
@@ -9626,7 +9626,7 @@
       <c r="I293" s="4"/>
       <c r="J293" s="4"/>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294" s="4" t="s">
         <v>358</v>
       </c>
@@ -9648,7 +9648,7 @@
       <c r="I294" s="4"/>
       <c r="J294" s="4"/>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295" s="4" t="s">
         <v>359</v>
       </c>
@@ -9668,7 +9668,7 @@
       <c r="I295" s="4"/>
       <c r="J295" s="4"/>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" s="4" t="s">
         <v>361</v>
       </c>
@@ -9688,7 +9688,7 @@
       <c r="I296" s="4"/>
       <c r="J296" s="4"/>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297" s="4" t="s">
         <v>362</v>
       </c>
@@ -9710,7 +9710,7 @@
       <c r="I297" s="4"/>
       <c r="J297" s="4"/>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298" s="4" t="s">
         <v>363</v>
       </c>
@@ -9742,7 +9742,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299" s="4" t="s">
         <v>364</v>
       </c>
@@ -9762,7 +9762,7 @@
       <c r="I299" s="4"/>
       <c r="J299" s="4"/>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300" s="4" t="s">
         <v>365</v>
       </c>
@@ -9790,7 +9790,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301" s="4" t="s">
         <v>366</v>
       </c>
@@ -9818,7 +9818,7 @@
       </c>
       <c r="J301" s="4"/>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302" s="4" t="s">
         <v>367</v>
       </c>
@@ -9842,7 +9842,7 @@
       <c r="I302" s="4"/>
       <c r="J302" s="4"/>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303" s="4" t="s">
         <v>368</v>
       </c>
@@ -9872,7 +9872,7 @@
       </c>
       <c r="J303" s="4"/>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304" s="4" t="s">
         <v>369</v>
       </c>
@@ -9894,7 +9894,7 @@
       <c r="I304" s="4"/>
       <c r="J304" s="4"/>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A305" s="4" t="s">
         <v>370</v>
       </c>
@@ -9922,7 +9922,7 @@
       </c>
       <c r="J305" s="4"/>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A306" s="4" t="s">
         <v>371</v>
       </c>
@@ -9948,7 +9948,7 @@
       <c r="I306" s="4"/>
       <c r="J306" s="4"/>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A307" s="4" t="s">
         <v>372</v>
       </c>
@@ -9978,7 +9978,7 @@
       </c>
       <c r="J307" s="4"/>
     </row>
-    <row r="308" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A308" s="4" t="s">
         <v>373</v>
       </c>
@@ -10010,7 +10010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A309" s="4" t="s">
         <v>374</v>
       </c>
@@ -10032,7 +10032,7 @@
       <c r="I309" s="4"/>
       <c r="J309" s="4"/>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A310" s="4" t="s">
         <v>375</v>
       </c>
@@ -10054,7 +10054,7 @@
       <c r="I310" s="4"/>
       <c r="J310" s="4"/>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311" s="7" t="s">
         <v>376</v>
       </c>
@@ -10076,7 +10076,7 @@
       <c r="I311" s="4"/>
       <c r="J311" s="37"/>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A312" s="7" t="s">
         <v>378</v>
       </c>
@@ -10098,7 +10098,7 @@
       <c r="I312" s="4"/>
       <c r="J312" s="37"/>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A313" s="4" t="s">
         <v>379</v>
       </c>
@@ -10122,7 +10122,7 @@
       <c r="I313" s="4"/>
       <c r="J313" s="37"/>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A314" s="4" t="s">
         <v>380</v>
       </c>
@@ -10144,7 +10144,7 @@
       <c r="I314" s="4"/>
       <c r="J314" s="37"/>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A315" s="4" t="s">
         <v>377</v>
       </c>
@@ -10166,7 +10166,7 @@
       <c r="I315" s="4"/>
       <c r="J315" s="37"/>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A316" s="4" t="s">
         <v>381</v>
       </c>
@@ -10188,7 +10188,7 @@
       <c r="I316" s="4"/>
       <c r="J316" s="37"/>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A317" s="4" t="s">
         <v>382</v>
       </c>
@@ -10210,7 +10210,7 @@
       <c r="I317" s="4"/>
       <c r="J317" s="37"/>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A318" s="4" t="s">
         <v>383</v>
       </c>
@@ -10230,7 +10230,7 @@
       <c r="I318" s="4"/>
       <c r="J318" s="37"/>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A319" s="4" t="s">
         <v>385</v>
       </c>
@@ -10252,7 +10252,7 @@
       <c r="I319" s="4"/>
       <c r="J319" s="37"/>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A320" s="4" t="s">
         <v>386</v>
       </c>
@@ -10274,7 +10274,7 @@
       <c r="I320" s="4"/>
       <c r="J320" s="37"/>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A321" s="4" t="s">
         <v>387</v>
       </c>
@@ -10296,7 +10296,7 @@
       <c r="I321" s="4"/>
       <c r="J321" s="37"/>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A322" s="4" t="s">
         <v>388</v>
       </c>
@@ -10318,7 +10318,7 @@
       <c r="I322" s="4"/>
       <c r="J322" s="4"/>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A323" s="4" t="s">
         <v>389</v>
       </c>
@@ -10340,7 +10340,7 @@
       <c r="I323" s="4"/>
       <c r="J323" s="4"/>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A324" s="4" t="s">
         <v>390</v>
       </c>
@@ -10362,7 +10362,7 @@
       <c r="I324" s="4"/>
       <c r="J324" s="4"/>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A325" s="4" t="s">
         <v>391</v>
       </c>
@@ -10380,7 +10380,7 @@
       <c r="I325" s="4"/>
       <c r="J325" s="4"/>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A326" s="4" t="s">
         <v>394</v>
       </c>
@@ -10402,7 +10402,7 @@
       <c r="I326" s="4"/>
       <c r="J326" s="4"/>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A327" s="4" t="s">
         <v>395</v>
       </c>
@@ -10426,7 +10426,7 @@
       <c r="I327" s="4"/>
       <c r="J327" s="4"/>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A328" s="4" t="s">
         <v>396</v>
       </c>
@@ -10446,7 +10446,7 @@
       <c r="I328" s="4"/>
       <c r="J328" s="4"/>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A329" s="4" t="s">
         <v>397</v>
       </c>
@@ -10466,7 +10466,7 @@
       <c r="I329" s="4"/>
       <c r="J329" s="4"/>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A330" s="4" t="s">
         <v>398</v>
       </c>
@@ -10498,7 +10498,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A331" s="4" t="s">
         <v>399</v>
       </c>
@@ -10526,7 +10526,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A332" s="4" t="s">
         <v>400</v>
       </c>
@@ -10552,7 +10552,7 @@
       </c>
       <c r="J332" s="4"/>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A333" s="4" t="s">
         <v>401</v>
       </c>
@@ -10576,7 +10576,7 @@
       <c r="I333" s="4"/>
       <c r="J333" s="4"/>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A334" s="4" t="s">
         <v>402</v>
       </c>
@@ -10598,7 +10598,7 @@
       <c r="I334" s="4"/>
       <c r="J334" s="4"/>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A335" s="4" t="s">
         <v>403</v>
       </c>
@@ -10616,7 +10616,7 @@
       <c r="I335" s="4"/>
       <c r="J335" s="4"/>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A336" s="4" t="s">
         <v>405</v>
       </c>
@@ -10638,7 +10638,7 @@
       <c r="I336" s="4"/>
       <c r="J336" s="4"/>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337" s="4" t="s">
         <v>407</v>
       </c>
@@ -10658,7 +10658,7 @@
       <c r="I337" s="4"/>
       <c r="J337" s="4"/>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338" s="4" t="s">
         <v>409</v>
       </c>
@@ -10678,7 +10678,7 @@
       <c r="I338" s="4"/>
       <c r="J338" s="4"/>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A339" s="4" t="s">
         <v>411</v>
       </c>
@@ -10698,7 +10698,7 @@
       <c r="I339" s="4"/>
       <c r="J339" s="4"/>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A340" s="4" t="s">
         <v>413</v>
       </c>
@@ -10720,7 +10720,7 @@
       <c r="I340" s="4"/>
       <c r="J340" s="4"/>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341" s="4" t="s">
         <v>414</v>
       </c>
@@ -10740,7 +10740,7 @@
       <c r="I341" s="4"/>
       <c r="J341" s="4"/>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342" s="4" t="s">
         <v>416</v>
       </c>
@@ -10762,7 +10762,7 @@
       <c r="I342" s="4"/>
       <c r="J342" s="4"/>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343" s="6" t="s">
         <v>624</v>
       </c>
@@ -10782,7 +10782,7 @@
       <c r="I343" s="4"/>
       <c r="J343" s="4"/>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344" s="4" t="s">
         <v>417</v>
       </c>
@@ -10802,7 +10802,7 @@
       <c r="I344" s="4"/>
       <c r="J344" s="4"/>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A345" s="4" t="s">
         <v>418</v>
       </c>
@@ -10822,7 +10822,7 @@
       <c r="I345" s="4"/>
       <c r="J345" s="4"/>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A346" s="4" t="s">
         <v>419</v>
       </c>
@@ -10842,7 +10842,7 @@
       <c r="I346" s="4"/>
       <c r="J346" s="4"/>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347" s="4" t="s">
         <v>420</v>
       </c>
@@ -10862,7 +10862,7 @@
       <c r="I347" s="4"/>
       <c r="J347" s="4"/>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348" s="4" t="s">
         <v>421</v>
       </c>
@@ -10882,7 +10882,7 @@
       <c r="I348" s="4"/>
       <c r="J348" s="4"/>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A349" s="4" t="s">
         <v>422</v>
       </c>
@@ -10902,7 +10902,7 @@
       <c r="I349" s="4"/>
       <c r="J349" s="4"/>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A350" s="4" t="s">
         <v>423</v>
       </c>
@@ -10922,7 +10922,7 @@
       <c r="I350" s="4"/>
       <c r="J350" s="4"/>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A351" s="4" t="s">
         <v>424</v>
       </c>
@@ -10940,7 +10940,7 @@
       <c r="I351" s="4"/>
       <c r="J351" s="4"/>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A352" s="4" t="s">
         <v>426</v>
       </c>
@@ -10960,7 +10960,7 @@
       <c r="I352" s="4"/>
       <c r="J352" s="4"/>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A353" s="4" t="s">
         <v>428</v>
       </c>
@@ -10980,7 +10980,7 @@
       <c r="I353" s="4"/>
       <c r="J353" s="4"/>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A354" s="4" t="s">
         <v>430</v>
       </c>
@@ -11000,7 +11000,7 @@
       <c r="I354" s="4"/>
       <c r="J354" s="4"/>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A355" s="4" t="s">
         <v>431</v>
       </c>
@@ -11018,7 +11018,7 @@
       <c r="I355" s="4"/>
       <c r="J355" s="4"/>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A356" s="4" t="s">
         <v>433</v>
       </c>
@@ -11040,7 +11040,7 @@
       <c r="I356" s="4"/>
       <c r="J356" s="4"/>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357" s="4" t="s">
         <v>435</v>
       </c>
@@ -11060,7 +11060,7 @@
       <c r="I357" s="4"/>
       <c r="J357" s="4"/>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A358" s="4" t="s">
         <v>621</v>
       </c>
@@ -11080,7 +11080,7 @@
       <c r="I358" s="4"/>
       <c r="J358" s="4"/>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A359" s="4" t="s">
         <v>436</v>
       </c>
@@ -11100,7 +11100,7 @@
       <c r="I359" s="4"/>
       <c r="J359" s="4"/>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A360" s="4" t="s">
         <v>437</v>
       </c>
@@ -11122,7 +11122,7 @@
       <c r="I360" s="4"/>
       <c r="J360" s="4"/>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A361" s="7" t="s">
         <v>438</v>
       </c>
@@ -11142,7 +11142,7 @@
       <c r="I361" s="4"/>
       <c r="J361" s="4"/>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A362" s="7" t="s">
         <v>440</v>
       </c>
@@ -11162,7 +11162,7 @@
       <c r="I362" s="4"/>
       <c r="J362" s="4"/>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A363" s="4" t="s">
         <v>441</v>
       </c>
@@ -11184,7 +11184,7 @@
       <c r="I363" s="4"/>
       <c r="J363" s="4"/>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A364" s="4" t="s">
         <v>442</v>
       </c>
@@ -11206,7 +11206,7 @@
       <c r="I364" s="4"/>
       <c r="J364" s="4"/>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A365" s="4" t="s">
         <v>444</v>
       </c>
@@ -11228,7 +11228,7 @@
       <c r="I365" s="4"/>
       <c r="J365" s="4"/>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A366" s="4" t="s">
         <v>445</v>
       </c>
@@ -11248,7 +11248,7 @@
       <c r="I366" s="4"/>
       <c r="J366" s="4"/>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A367" s="4" t="s">
         <v>447</v>
       </c>
@@ -11268,7 +11268,7 @@
       <c r="I367" s="4"/>
       <c r="J367" s="4"/>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A368" s="4" t="s">
         <v>504</v>
       </c>
@@ -11288,7 +11288,7 @@
       <c r="I368" s="4"/>
       <c r="J368" s="4"/>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A369" s="7" t="s">
         <v>448</v>
       </c>
@@ -11308,7 +11308,7 @@
       <c r="I369" s="4"/>
       <c r="J369" s="4"/>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A370" s="4" t="s">
         <v>449</v>
       </c>
@@ -11330,7 +11330,7 @@
       <c r="I370" s="4"/>
       <c r="J370" s="4"/>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A371" s="4" t="s">
         <v>450</v>
       </c>
@@ -11350,7 +11350,7 @@
       <c r="I371" s="4"/>
       <c r="J371" s="4"/>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A372" s="4" t="s">
         <v>451</v>
       </c>
@@ -11372,7 +11372,7 @@
       <c r="I372" s="4"/>
       <c r="J372" s="4"/>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A373" s="4" t="s">
         <v>453</v>
       </c>
@@ -11392,7 +11392,7 @@
       <c r="I373" s="4"/>
       <c r="J373" s="4"/>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A374" s="4" t="s">
         <v>455</v>
       </c>
@@ -11412,7 +11412,7 @@
       <c r="I374" s="4"/>
       <c r="J374" s="4"/>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A375" s="4" t="s">
         <v>456</v>
       </c>
@@ -11434,7 +11434,7 @@
       <c r="I375" s="4"/>
       <c r="J375" s="4"/>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A376" s="4" t="s">
         <v>457</v>
       </c>
@@ -11456,7 +11456,7 @@
       <c r="I376" s="4"/>
       <c r="J376" s="4"/>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A377" s="4" t="s">
         <v>458</v>
       </c>
@@ -11476,7 +11476,7 @@
       <c r="I377" s="4"/>
       <c r="J377" s="4"/>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A378" s="4" t="s">
         <v>460</v>
       </c>
@@ -11496,7 +11496,7 @@
       <c r="I378" s="4"/>
       <c r="J378" s="4"/>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A379" s="4" t="s">
         <v>611</v>
       </c>
@@ -11516,7 +11516,7 @@
       <c r="I379" s="4"/>
       <c r="J379" s="4"/>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A380" s="4" t="s">
         <v>461</v>
       </c>
@@ -11536,7 +11536,7 @@
       <c r="I380" s="4"/>
       <c r="J380" s="4"/>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A381" s="4" t="s">
         <v>462</v>
       </c>
@@ -11556,7 +11556,7 @@
       <c r="I381" s="4"/>
       <c r="J381" s="4"/>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A382" s="7" t="s">
         <v>464</v>
       </c>
@@ -11576,7 +11576,7 @@
       <c r="I382" s="4"/>
       <c r="J382" s="4"/>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A383" s="4" t="s">
         <v>465</v>
       </c>
@@ -11596,7 +11596,7 @@
       <c r="I383" s="4"/>
       <c r="J383" s="4"/>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A384" s="4" t="s">
         <v>466</v>
       </c>
@@ -11616,7 +11616,7 @@
       <c r="I384" s="4"/>
       <c r="J384" s="4"/>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A385" s="4" t="s">
         <v>467</v>
       </c>
@@ -11634,7 +11634,7 @@
       <c r="I385" s="4"/>
       <c r="J385" s="4"/>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A386" s="4" t="s">
         <v>469</v>
       </c>
@@ -11656,7 +11656,7 @@
       <c r="I386" s="4"/>
       <c r="J386" s="4"/>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A387" s="4" t="s">
         <v>471</v>
       </c>
@@ -11674,7 +11674,7 @@
       <c r="I387" s="4"/>
       <c r="J387" s="4"/>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A388" s="4" t="s">
         <v>473</v>
       </c>
@@ -11696,7 +11696,7 @@
       <c r="I388" s="4"/>
       <c r="J388" s="4"/>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A389" s="4" t="s">
         <v>475</v>
       </c>
@@ -11718,7 +11718,7 @@
       <c r="I389" s="4"/>
       <c r="J389" s="4"/>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A390" s="4" t="s">
         <v>476</v>
       </c>
@@ -11740,7 +11740,7 @@
       <c r="I390" s="4"/>
       <c r="J390" s="4"/>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A391" s="4" t="s">
         <v>477</v>
       </c>
@@ -11762,7 +11762,7 @@
       <c r="I391" s="4"/>
       <c r="J391" s="4"/>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A392" s="4" t="s">
         <v>478</v>
       </c>
@@ -11784,7 +11784,7 @@
       <c r="I392" s="4"/>
       <c r="J392" s="4"/>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A393" s="4" t="s">
         <v>479</v>
       </c>
@@ -11806,7 +11806,7 @@
       <c r="I393" s="4"/>
       <c r="J393" s="4"/>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A394" s="4" t="s">
         <v>480</v>
       </c>
@@ -11824,7 +11824,7 @@
       <c r="I394" s="4"/>
       <c r="J394" s="4"/>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A395" s="4" t="s">
         <v>482</v>
       </c>
@@ -11846,7 +11846,7 @@
       <c r="I395" s="4"/>
       <c r="J395" s="4"/>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A396" s="4" t="s">
         <v>484</v>
       </c>
@@ -11866,7 +11866,7 @@
       <c r="I396" s="4"/>
       <c r="J396" s="4"/>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A397" s="4" t="s">
         <v>614</v>
       </c>
@@ -11886,7 +11886,7 @@
       <c r="I397" s="4"/>
       <c r="J397" s="4"/>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A398" s="4" t="s">
         <v>486</v>
       </c>
@@ -11908,7 +11908,7 @@
       <c r="I398" s="4"/>
       <c r="J398" s="4"/>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A399" s="4" t="s">
         <v>487</v>
       </c>
@@ -11930,7 +11930,7 @@
       <c r="I399" s="4"/>
       <c r="J399" s="4"/>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A400" s="4" t="s">
         <v>488</v>
       </c>
@@ -11952,7 +11952,7 @@
       <c r="I400" s="4"/>
       <c r="J400" s="4"/>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A401" s="4" t="s">
         <v>490</v>
       </c>
@@ -11974,7 +11974,7 @@
       <c r="I401" s="4"/>
       <c r="J401" s="4"/>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A402" s="4" t="s">
         <v>491</v>
       </c>
@@ -11996,7 +11996,7 @@
       <c r="I402" s="4"/>
       <c r="J402" s="4"/>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A403" s="4" t="s">
         <v>492</v>
       </c>
@@ -12018,7 +12018,7 @@
       <c r="I403" s="4"/>
       <c r="J403" s="4"/>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A404" s="4" t="s">
         <v>494</v>
       </c>
@@ -12036,7 +12036,7 @@
       <c r="I404" s="4"/>
       <c r="J404" s="4"/>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A405" s="4" t="s">
         <v>496</v>
       </c>
@@ -12058,7 +12058,7 @@
       <c r="I405" s="4"/>
       <c r="J405" s="4"/>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A406" s="4" t="s">
         <v>498</v>
       </c>
@@ -12080,7 +12080,7 @@
       <c r="I406" s="4"/>
       <c r="J406" s="4"/>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A407" s="4" t="s">
         <v>499</v>
       </c>
@@ -12102,7 +12102,7 @@
       <c r="I407" s="4"/>
       <c r="J407" s="4"/>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A408" s="4" t="s">
         <v>500</v>
       </c>
@@ -12124,7 +12124,7 @@
       <c r="I408" s="4"/>
       <c r="J408" s="4"/>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A409" s="4" t="s">
         <v>502</v>
       </c>
@@ -12146,7 +12146,7 @@
       <c r="I409" s="4"/>
       <c r="J409" s="4"/>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A410" s="4" t="s">
         <v>503</v>
       </c>
@@ -12166,7 +12166,7 @@
       <c r="I410" s="4"/>
       <c r="J410" s="4"/>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A411" s="4" t="s">
         <v>506</v>
       </c>
@@ -12188,7 +12188,7 @@
       <c r="I411" s="4"/>
       <c r="J411" s="4"/>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A412" s="4" t="s">
         <v>508</v>
       </c>
@@ -12210,7 +12210,7 @@
       <c r="I412" s="4"/>
       <c r="J412" s="4"/>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A413" s="4" t="s">
         <v>509</v>
       </c>
@@ -12232,7 +12232,7 @@
       <c r="I413" s="4"/>
       <c r="J413" s="4"/>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A414" s="4" t="s">
         <v>510</v>
       </c>
@@ -12254,7 +12254,7 @@
       <c r="I414" s="4"/>
       <c r="J414" s="4"/>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A415" s="4" t="s">
         <v>511</v>
       </c>
@@ -12272,7 +12272,7 @@
       <c r="I415" s="4"/>
       <c r="J415" s="4"/>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A416" s="4" t="s">
         <v>507</v>
       </c>
@@ -12294,7 +12294,7 @@
       <c r="I416" s="4"/>
       <c r="J416" s="4"/>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A417" s="4" t="s">
         <v>513</v>
       </c>
@@ -12314,7 +12314,7 @@
       <c r="I417" s="4"/>
       <c r="J417" s="4"/>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A418" s="4" t="s">
         <v>516</v>
       </c>
@@ -12336,7 +12336,7 @@
       <c r="I418" s="4"/>
       <c r="J418" s="4"/>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A419" s="4" t="s">
         <v>517</v>
       </c>
@@ -12358,7 +12358,7 @@
       <c r="I419" s="4"/>
       <c r="J419" s="4"/>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A420" s="4" t="s">
         <v>518</v>
       </c>
@@ -12380,7 +12380,7 @@
       <c r="I420" s="4"/>
       <c r="J420" s="4"/>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A421" s="4" t="s">
         <v>520</v>
       </c>
@@ -12398,7 +12398,7 @@
       <c r="I421" s="4"/>
       <c r="J421" s="4"/>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A422" s="4" t="s">
         <v>522</v>
       </c>
@@ -12418,7 +12418,7 @@
       <c r="I422" s="4"/>
       <c r="J422" s="4"/>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A423" s="4" t="s">
         <v>524</v>
       </c>
@@ -12440,7 +12440,7 @@
       <c r="I423" s="4"/>
       <c r="J423" s="4"/>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A424" s="4" t="s">
         <v>525</v>
       </c>
@@ -12466,7 +12466,7 @@
       <c r="I424" s="4"/>
       <c r="J424" s="4"/>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A425" s="4" t="s">
         <v>526</v>
       </c>
@@ -12488,7 +12488,7 @@
       <c r="I425" s="4"/>
       <c r="J425" s="4"/>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A426" s="4" t="s">
         <v>527</v>
       </c>
@@ -12508,7 +12508,7 @@
       <c r="I426" s="4"/>
       <c r="J426" s="4"/>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A427" s="4" t="s">
         <v>528</v>
       </c>
@@ -12540,7 +12540,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A428" s="4" t="s">
         <v>529</v>
       </c>
@@ -12562,7 +12562,7 @@
       <c r="I428" s="4"/>
       <c r="J428" s="4"/>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A429" s="4" t="s">
         <v>530</v>
       </c>
@@ -12584,7 +12584,7 @@
       <c r="I429" s="4"/>
       <c r="J429" s="4"/>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A430" s="4" t="s">
         <v>531</v>
       </c>
@@ -12602,7 +12602,7 @@
       <c r="I430" s="4"/>
       <c r="J430" s="4"/>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A431" s="4" t="s">
         <v>532</v>
       </c>
@@ -12620,7 +12620,7 @@
       <c r="I431" s="4"/>
       <c r="J431" s="4"/>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A432" s="4" t="s">
         <v>534</v>
       </c>
@@ -12638,7 +12638,7 @@
       <c r="I432" s="4"/>
       <c r="J432" s="4"/>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A433" s="4" t="s">
         <v>536</v>
       </c>
@@ -12654,7 +12654,7 @@
       <c r="I433" s="4"/>
       <c r="J433" s="4"/>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A434" s="4" t="s">
         <v>537</v>
       </c>
@@ -12670,7 +12670,7 @@
       <c r="I434" s="4"/>
       <c r="J434" s="4"/>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A435" s="7" t="s">
         <v>538</v>
       </c>
@@ -12690,7 +12690,7 @@
       <c r="I435" s="4"/>
       <c r="J435" s="4"/>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A436" s="4" t="s">
         <v>539</v>
       </c>
@@ -12712,7 +12712,7 @@
       </c>
       <c r="J436" s="4"/>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A437" s="4" t="s">
         <v>541</v>
       </c>
@@ -12734,7 +12734,7 @@
       <c r="I437" s="4"/>
       <c r="J437" s="4"/>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A438" s="4" t="s">
         <v>542</v>
       </c>
@@ -12764,7 +12764,7 @@
       </c>
       <c r="J438" s="4"/>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A439" s="4" t="s">
         <v>543</v>
       </c>
@@ -12786,7 +12786,7 @@
       </c>
       <c r="J439" s="4"/>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A440" s="4" t="s">
         <v>545</v>
       </c>
@@ -12808,7 +12808,7 @@
       <c r="I440" s="4"/>
       <c r="J440" s="4"/>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A441" s="4" t="s">
         <v>547</v>
       </c>
@@ -12828,7 +12828,7 @@
       <c r="I441" s="4"/>
       <c r="J441" s="4"/>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A442" s="4" t="s">
         <v>549</v>
       </c>
@@ -12848,7 +12848,7 @@
       <c r="I442" s="4"/>
       <c r="J442" s="4"/>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A443" s="4" t="s">
         <v>551</v>
       </c>
@@ -12874,7 +12874,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A444" s="4" t="s">
         <v>553</v>
       </c>
@@ -12894,7 +12894,7 @@
       <c r="I444" s="4"/>
       <c r="J444" s="4"/>
     </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A445" s="4" t="s">
         <v>555</v>
       </c>
@@ -12916,7 +12916,7 @@
       <c r="I445" s="4"/>
       <c r="J445" s="4"/>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A446" s="4" t="s">
         <v>552</v>
       </c>
@@ -12938,7 +12938,7 @@
       <c r="I446" s="4"/>
       <c r="J446" s="4"/>
     </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A447" s="4" t="s">
         <v>556</v>
       </c>
@@ -12958,7 +12958,7 @@
       <c r="I447" s="4"/>
       <c r="J447" s="4"/>
     </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A448" s="4" t="s">
         <v>557</v>
       </c>
@@ -12978,7 +12978,7 @@
       <c r="I448" s="4"/>
       <c r="J448" s="4"/>
     </row>
-    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A449" s="4" t="s">
         <v>559</v>
       </c>
@@ -13002,7 +13002,7 @@
       <c r="I449" s="4"/>
       <c r="J449" s="4"/>
     </row>
-    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A450" s="4" t="s">
         <v>560</v>
       </c>
@@ -13022,7 +13022,7 @@
       <c r="I450" s="4"/>
       <c r="J450" s="4"/>
     </row>
-    <row r="451" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A451" s="4" t="s">
         <v>561</v>
       </c>
@@ -13042,7 +13042,7 @@
       <c r="I451" s="4"/>
       <c r="J451" s="4"/>
     </row>
-    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A452" s="4" t="s">
         <v>563</v>
       </c>
@@ -13062,7 +13062,7 @@
       <c r="I452" s="4"/>
       <c r="J452" s="4"/>
     </row>
-    <row r="453" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A453" s="4" t="s">
         <v>565</v>
       </c>
@@ -13084,7 +13084,7 @@
       <c r="I453" s="4"/>
       <c r="J453" s="4"/>
     </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A454" s="7" t="s">
         <v>566</v>
       </c>
@@ -13104,7 +13104,7 @@
       <c r="I454" s="4"/>
       <c r="J454" s="4"/>
     </row>
-    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A455" s="7" t="s">
         <v>568</v>
       </c>
@@ -13124,7 +13124,7 @@
       <c r="I455" s="4"/>
       <c r="J455" s="4"/>
     </row>
-    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A456" s="4" t="s">
         <v>570</v>
       </c>
@@ -13156,7 +13156,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="457" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A457" s="4" t="s">
         <v>571</v>
       </c>
@@ -13176,7 +13176,7 @@
       <c r="I457" s="4"/>
       <c r="J457" s="4"/>
     </row>
-    <row r="458" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A458" s="4" t="s">
         <v>572</v>
       </c>
@@ -13208,7 +13208,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A459" s="4" t="s">
         <v>573</v>
       </c>
@@ -13236,7 +13236,7 @@
       </c>
       <c r="J459" s="4"/>
     </row>
-    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A460" s="4" t="s">
         <v>574</v>
       </c>
@@ -13266,7 +13266,7 @@
       </c>
       <c r="J460" s="4"/>
     </row>
-    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A461" s="4" t="s">
         <v>575</v>
       </c>
@@ -13288,7 +13288,7 @@
       <c r="I461" s="4"/>
       <c r="J461" s="4"/>
     </row>
-    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A462" s="4" t="s">
         <v>576</v>
       </c>
@@ -13318,7 +13318,7 @@
       </c>
       <c r="J462" s="4"/>
     </row>
-    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A463" s="4" t="s">
         <v>577</v>
       </c>
@@ -13342,7 +13342,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="464" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A464" s="4" t="s">
         <v>578</v>
       </c>
@@ -13362,7 +13362,7 @@
       <c r="I464" s="4"/>
       <c r="J464" s="4"/>
     </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A465" s="4" t="s">
         <v>579</v>
       </c>
@@ -13392,7 +13392,7 @@
       </c>
       <c r="J465" s="4"/>
     </row>
-    <row r="466" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A466" s="4" t="s">
         <v>580</v>
       </c>
@@ -13414,7 +13414,7 @@
       <c r="I466" s="4"/>
       <c r="J466" s="4"/>
     </row>
-    <row r="467" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A467" s="4" t="s">
         <v>581</v>
       </c>
@@ -13446,7 +13446,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A468" s="4" t="s">
         <v>582</v>
       </c>
@@ -13470,7 +13470,7 @@
       </c>
       <c r="J468" s="4"/>
     </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A469" s="4" t="s">
         <v>583</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="470" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A470" s="4" t="s">
         <v>585</v>
       </c>
@@ -13518,7 +13518,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="471" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A471" s="21" t="s">
         <v>586</v>
       </c>
@@ -13542,7 +13542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="472" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A472" s="4" t="s">
         <v>587</v>
       </c>
@@ -13570,7 +13570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A473" s="22" t="s">
         <v>588</v>
       </c>
@@ -13588,7 +13588,7 @@
       <c r="I473" s="24"/>
       <c r="J473" s="23"/>
     </row>
-    <row r="474" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A474" s="18" t="s">
         <v>266</v>
       </c>
@@ -13608,7 +13608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A475" s="7" t="s">
         <v>269</v>
       </c>
@@ -13626,7 +13626,7 @@
       <c r="I475" s="4"/>
       <c r="J475" s="4"/>
     </row>
-    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A476" s="4" t="s">
         <v>274</v>
       </c>
@@ -13644,7 +13644,7 @@
       <c r="I476" s="4"/>
       <c r="J476" s="4"/>
     </row>
-    <row r="477" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A477" s="4" t="s">
         <v>277</v>
       </c>
@@ -13662,7 +13662,7 @@
       <c r="I477" s="4"/>
       <c r="J477" s="4"/>
     </row>
-    <row r="478" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A478" s="7" t="s">
         <v>278</v>
       </c>
@@ -13680,7 +13680,7 @@
       <c r="I478" s="4"/>
       <c r="J478" s="4"/>
     </row>
-    <row r="479" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A479" s="18" t="s">
         <v>608</v>
       </c>
@@ -13698,7 +13698,7 @@
       <c r="I479" s="4"/>
       <c r="J479" s="4"/>
     </row>
-    <row r="480" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A480" s="4" t="s">
         <v>293</v>
       </c>
@@ -13716,7 +13716,7 @@
       <c r="I480" s="4"/>
       <c r="J480" s="4"/>
     </row>
-    <row r="481" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A481" s="4" t="s">
         <v>590</v>
       </c>
@@ -13730,7 +13730,7 @@
       <c r="I481" s="25"/>
       <c r="J481" s="25"/>
     </row>
-    <row r="482" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A482" s="4" t="s">
         <v>591</v>
       </c>
@@ -13744,7 +13744,7 @@
       <c r="I482" s="25"/>
       <c r="J482" s="25"/>
     </row>
-    <row r="483" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A483" s="4" t="s">
         <v>592</v>
       </c>
@@ -13758,7 +13758,7 @@
       <c r="I483" s="25"/>
       <c r="J483" s="25"/>
     </row>
-    <row r="484" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A484" s="4" t="s">
         <v>593</v>
       </c>
@@ -13772,7 +13772,7 @@
       <c r="I484" s="25"/>
       <c r="J484" s="25"/>
     </row>
-    <row r="485" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A485" s="4" t="s">
         <v>594</v>
       </c>
@@ -13786,7 +13786,7 @@
       <c r="I485" s="25"/>
       <c r="J485" s="25"/>
     </row>
-    <row r="486" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A486" s="4" t="s">
         <v>595</v>
       </c>
@@ -13800,7 +13800,7 @@
       <c r="I486" s="25"/>
       <c r="J486" s="25"/>
     </row>
-    <row r="487" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A487" s="4" t="s">
         <v>596</v>
       </c>
@@ -13814,7 +13814,7 @@
       <c r="I487" s="25"/>
       <c r="J487" s="25"/>
     </row>
-    <row r="488" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A488" s="4" t="s">
         <v>597</v>
       </c>
@@ -13828,7 +13828,7 @@
       <c r="I488" s="25"/>
       <c r="J488" s="25"/>
     </row>
-    <row r="489" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A489" s="4" t="s">
         <v>598</v>
       </c>
@@ -13842,7 +13842,7 @@
       <c r="I489" s="25"/>
       <c r="J489" s="25"/>
     </row>
-    <row r="490" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A490" s="4" t="s">
         <v>599</v>
       </c>
@@ -13856,7 +13856,7 @@
       <c r="I490" s="25"/>
       <c r="J490" s="25"/>
     </row>
-    <row r="491" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A491" s="4" t="s">
         <v>600</v>
       </c>
@@ -13870,7 +13870,7 @@
       <c r="I491" s="25"/>
       <c r="J491" s="25"/>
     </row>
-    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A492" s="4" t="s">
         <v>601</v>
       </c>
@@ -13884,7 +13884,7 @@
       <c r="I492" s="25"/>
       <c r="J492" s="25"/>
     </row>
-    <row r="493" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A493" s="4" t="s">
         <v>602</v>
       </c>
@@ -13898,7 +13898,7 @@
       <c r="I493" s="25"/>
       <c r="J493" s="25"/>
     </row>
-    <row r="494" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A494" s="4" t="s">
         <v>603</v>
       </c>
@@ -13912,7 +13912,7 @@
       <c r="I494" s="25"/>
       <c r="J494" s="25"/>
     </row>
-    <row r="495" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A495" s="4" t="s">
         <v>604</v>
       </c>
@@ -13926,7 +13926,7 @@
       <c r="I495" s="25"/>
       <c r="J495" s="25"/>
     </row>
-    <row r="496" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A496" s="4" t="s">
         <v>605</v>
       </c>
@@ -13940,7 +13940,7 @@
       <c r="I496" s="25"/>
       <c r="J496" s="25"/>
     </row>
-    <row r="497" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A497" s="4" t="s">
         <v>606</v>
       </c>
@@ -13953,7 +13953,7 @@
       <c r="I497" s="25"/>
       <c r="J497" s="25"/>
     </row>
-    <row r="498" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A498" s="4" t="s">
         <v>607</v>
       </c>
@@ -13971,9 +13971,9 @@
   <phoneticPr fontId="23" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.17" right="0.17" top="0.47" bottom="0.57999999999999996" header="0" footer="0"/>
-  <pageSetup paperSize="5" scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="89" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;F&amp;C&amp;P&amp;ROctober 22, 2024</oddFooter>
+    <oddFooter>&amp;L&amp;F&amp;C&amp;P&amp;RNovember 15, 2024</oddFooter>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>